<commit_message>
Created repository and controller for users on a web service with UI for registration activity and webservice module for web service calls from android. Created initial file for specifications and changed scrum tables effort values
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>New estimates of effort remaining as of sprint</t>
   </si>
@@ -103,12 +103,24 @@
     <t>Tomislav</t>
   </si>
   <si>
-    <t>izraditi ERA model</t>
+    <t>osigurati server</t>
   </si>
   <si>
     <t>Leon</t>
   </si>
   <si>
+    <t>instalirati potrebne programe na serveru</t>
+  </si>
+  <si>
+    <t>izraditi ERA model i prenesti na bazu</t>
+  </si>
+  <si>
+    <t>Izraditi web service modul za android</t>
+  </si>
+  <si>
+    <t>Maja &amp; Tomislav</t>
+  </si>
+  <si>
     <t>napraviti activity za prijavu (UI)</t>
   </si>
   <si>
@@ -143,17 +155,24 @@
   </si>
   <si>
     <t>napraviti logiku web servisa za izmjenu profila</t>
+  </si>
+  <si>
+    <t>Burndown chart vrijednosti – ideal</t>
+  </si>
+  <si>
+    <t>Burndown chart vrijednosti – stvarno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
+    <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -190,6 +209,31 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -213,7 +257,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6D9F1"/>
-        <bgColor rgb="FFC0C0C0"/>
+        <bgColor rgb="FF99CCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -356,7 +400,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,6 +477,18 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,11 +509,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -486,7 +546,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -517,7 +577,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF002060"/>
@@ -526,11 +586,548 @@
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF004586"/>
       <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1" sz="1300">
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Burndown chart</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>ideal</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1 backlog'!$D$2:$W$2</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Initial estimate of effort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10/20/2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10/21/2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10/22/2015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10/23/2015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10/24/2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10/25/2015</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10/26/2015</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10/27/2015</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10/28/2015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10/29/2015</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10/30/2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10/31/2015</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11/1/2015</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11/2/2015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11/3/2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11/4/2015</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11/5/2015</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11/6/2015</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11/7/2015</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1 backlog'!$D$18:$W$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.4210526315789</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.8421052631579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.2631578947368</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.6842105263158</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.1052631578947</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.5263157894737</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.9473684210526</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>17.3684210526316</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.7894736842105</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>14.2105263157895</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12.6315789473684</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.0526315789474</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.47368421052632</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7.89473684210527</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>6.31578947368422</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.73684210526316</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.15789473684211</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.57894736842106</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>6.66133814775094E-015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>current</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>current</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:size val="6"/>
+          </c:marker>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Sprint 1 backlog'!$D$2:$W$2</c:f>
+              <c:strCache>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>Initial estimate of effort</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10/20/2015</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10/21/2015</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10/22/2015</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10/23/2015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10/24/2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10/25/2015</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10/26/2015</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10/27/2015</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10/28/2015</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10/29/2015</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10/30/2015</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10/31/2015</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11/1/2015</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11/2/2015</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11/3/2015</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11/4/2015</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11/5/2015</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>11/6/2015</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>11/7/2015</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 1 backlog'!$D$19:$W$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="93854753"/>
+        <c:axId val="16893701"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="93854753"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Date</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="16893701"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="16893701"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Effort</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="none"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="93854753"/>
+        <c:crossesAt val="1"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1775160</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>117360</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>936720</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>152280</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="1775160" y="6534000"/>
+        <a:ext cx="10136160" cy="4987800"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -541,7 +1138,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -593,7 +1190,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -604,7 +1201,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="6" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -926,10 +1523,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1057,13 +1654,65 @@
       <c r="D3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E3" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V3" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W3" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18"/>
       <c r="B4" s="6" t="s">
         <v>26</v>
@@ -1074,13 +1723,65 @@
       <c r="D4" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E4" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18"/>
       <c r="B5" s="6" t="s">
         <v>28</v>
@@ -1091,53 +1792,119 @@
       <c r="D5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="18"/>
       <c r="B6" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E6" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E6" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="18"/>
-      <c r="B7" s="19" t="s">
-        <v>32</v>
+      <c r="B7" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E7" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="18"/>
       <c r="B8" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>2</v>
@@ -1145,169 +1912,553 @@
       <c r="E8" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="18"/>
       <c r="B9" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="D9" s="6" t="n">
         <v>2</v>
       </c>
       <c r="E9" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F9" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="18"/>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="22" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E10" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="F10" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18"/>
       <c r="B11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="21" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="19" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="18"/>
+      <c r="B12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="6" t="n">
+      <c r="D12" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="18"/>
+      <c r="B13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="28.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="18"/>
+      <c r="B14" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E14" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="s">
+      <c r="F14" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="T14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V14" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W14" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="28.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="21" t="s">
+      <c r="B15" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="21" t="n">
+      <c r="D15" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="E12" s="21" t="n">
+      <c r="E15" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="22"/>
-      <c r="W12" s="22"/>
-      <c r="X12" s="22"/>
-    </row>
-    <row r="13" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18"/>
-      <c r="B13" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="24" t="s">
+      <c r="F15" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="24" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="25"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="25"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25"/>
+    </row>
+    <row r="16" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="18"/>
+      <c r="B16" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="24" t="n">
+      <c r="D16" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="E13" s="24" t="n">
+      <c r="E16" s="22" t="n">
         <v>3</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="25"/>
-      <c r="S13" s="25"/>
-      <c r="T13" s="25"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="25"/>
-      <c r="W13" s="25"/>
-      <c r="X13" s="25"/>
-    </row>
-    <row r="14" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18"/>
-      <c r="B14" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="24" t="s">
+      <c r="F16" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="22" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="I16" s="27"/>
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
+      <c r="R16" s="27"/>
+      <c r="S16" s="27"/>
+      <c r="T16" s="27"/>
+      <c r="U16" s="27"/>
+      <c r="V16" s="27"/>
+      <c r="W16" s="27"/>
+      <c r="X16" s="27"/>
+    </row>
+    <row r="17" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="18"/>
+      <c r="B17" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="24" t="n">
+      <c r="D17" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="E14" s="24" t="n">
+      <c r="E17" s="22" t="n">
         <v>1</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
-      <c r="T14" s="25"/>
-      <c r="U14" s="25"/>
-      <c r="V14" s="25"/>
-      <c r="W14" s="25"/>
-      <c r="X14" s="25"/>
+      <c r="F17" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="22" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="27"/>
+      <c r="T17" s="27"/>
+      <c r="U17" s="27"/>
+      <c r="V17" s="27"/>
+      <c r="W17" s="27"/>
+      <c r="X17" s="27"/>
+    </row>
+    <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="0" t="n">
+        <f aca="false">SUM(D3:D17)</f>
+        <v>30</v>
+      </c>
+      <c r="E18" s="29" t="n">
+        <f aca="false">D18-($D$18/19)</f>
+        <v>28.4210526315789</v>
+      </c>
+      <c r="F18" s="29" t="n">
+        <f aca="false">E18-($D$18/19)</f>
+        <v>26.8421052631579</v>
+      </c>
+      <c r="G18" s="29" t="n">
+        <f aca="false">F18-($D$18/19)</f>
+        <v>25.2631578947368</v>
+      </c>
+      <c r="H18" s="29" t="n">
+        <f aca="false">G18-($D$18/19)</f>
+        <v>23.6842105263158</v>
+      </c>
+      <c r="I18" s="29" t="n">
+        <f aca="false">H18-($D$18/19)</f>
+        <v>22.1052631578947</v>
+      </c>
+      <c r="J18" s="29" t="n">
+        <f aca="false">I18-($D$18/19)</f>
+        <v>20.5263157894737</v>
+      </c>
+      <c r="K18" s="29" t="n">
+        <f aca="false">J18-($D$18/19)</f>
+        <v>18.9473684210526</v>
+      </c>
+      <c r="L18" s="29" t="n">
+        <f aca="false">K18-($D$18/19)</f>
+        <v>17.3684210526316</v>
+      </c>
+      <c r="M18" s="29" t="n">
+        <f aca="false">L18-($D$18/19)</f>
+        <v>15.7894736842105</v>
+      </c>
+      <c r="N18" s="29" t="n">
+        <f aca="false">M18-($D$18/19)</f>
+        <v>14.2105263157895</v>
+      </c>
+      <c r="O18" s="29" t="n">
+        <f aca="false">N18-($D$18/19)</f>
+        <v>12.6315789473684</v>
+      </c>
+      <c r="P18" s="29" t="n">
+        <f aca="false">O18-($D$18/19)</f>
+        <v>11.0526315789474</v>
+      </c>
+      <c r="Q18" s="29" t="n">
+        <f aca="false">P18-($D$18/19)</f>
+        <v>9.47368421052632</v>
+      </c>
+      <c r="R18" s="29" t="n">
+        <f aca="false">Q18-($D$18/19)</f>
+        <v>7.89473684210527</v>
+      </c>
+      <c r="S18" s="29" t="n">
+        <f aca="false">R18-($D$18/19)</f>
+        <v>6.31578947368422</v>
+      </c>
+      <c r="T18" s="29" t="n">
+        <f aca="false">S18-($D$18/19)</f>
+        <v>4.73684210526316</v>
+      </c>
+      <c r="U18" s="29" t="n">
+        <f aca="false">T18-($D$18/19)</f>
+        <v>3.15789473684211</v>
+      </c>
+      <c r="V18" s="29" t="n">
+        <f aca="false">U18-($D$18/19)</f>
+        <v>1.57894736842106</v>
+      </c>
+      <c r="W18" s="29" t="n">
+        <f aca="false">V18-($D$18/19)</f>
+        <v>6.66133814775094E-015</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="30.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="0" t="n">
+        <f aca="false">SUM(D3:D17)</f>
+        <v>30</v>
+      </c>
+      <c r="E19" s="0" t="n">
+        <f aca="false">SUM(E3:E17)</f>
+        <v>28</v>
+      </c>
+      <c r="F19" s="0" t="n">
+        <f aca="false">SUM(F3:F17)</f>
+        <v>28</v>
+      </c>
+      <c r="G19" s="0" t="n">
+        <f aca="false">SUM(G3:G17)</f>
+        <v>25</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">SUM(H3:H17)</f>
+        <v>20</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <f aca="false">SUM(I3:I17)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <f aca="false">SUM(J3:J17)</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <f aca="false">SUM(K3:K17)</f>
+        <v>0</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <f aca="false">SUM(L3:L17)</f>
+        <v>0</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <f aca="false">SUM(M3:M17)</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="0" t="n">
+        <f aca="false">SUM(N3:N17)</f>
+        <v>0</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <f aca="false">SUM(O3:O17)</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="0" t="n">
+        <f aca="false">SUM(P3:P17)</f>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="0" t="n">
+        <f aca="false">SUM(Q3:Q17)</f>
+        <v>0</v>
+      </c>
+      <c r="R19" s="0" t="n">
+        <f aca="false">SUM(R3:R17)</f>
+        <v>0</v>
+      </c>
+      <c r="S19" s="0" t="n">
+        <f aca="false">SUM(S3:S17)</f>
+        <v>0</v>
+      </c>
+      <c r="T19" s="0" t="n">
+        <f aca="false">SUM(T3:T17)</f>
+        <v>0</v>
+      </c>
+      <c r="U19" s="0" t="n">
+        <f aca="false">SUM(U3:U17)</f>
+        <v>0</v>
+      </c>
+      <c r="V19" s="0" t="n">
+        <f aca="false">SUM(V3:V17)</f>
+        <v>0</v>
+      </c>
+      <c r="W19" s="0" t="n">
+        <f aca="false">SUM(W3:W17)</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="E1:X1"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A19:C19"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1316,5 +2467,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated scrum tables for day 2015-10-28
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -241,8 +241,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -418,7 +417,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -519,10 +518,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -560,10 +555,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -704,7 +695,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -877,7 +868,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="3"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -988,7 +979,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0</c:v>
@@ -1025,11 +1016,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="97463697"/>
-        <c:axId val="7069963"/>
+        <c:axId val="51489986"/>
+        <c:axId val="74616764"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="97463697"/>
+        <c:axId val="51489986"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1069,14 +1060,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="7069963"/>
+        <c:crossAx val="74616764"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7069963"/>
+        <c:axId val="74616764"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1126,7 +1117,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="97463697"/>
+        <c:crossAx val="51489986"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1166,15 +1157,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1829160</xdr:colOff>
+      <xdr:colOff>1856160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>135720</xdr:rowOff>
+      <xdr:rowOff>126720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>824040</xdr:colOff>
+      <xdr:colOff>850680</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>48600</xdr:rowOff>
+      <xdr:rowOff>39240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1182,8 +1173,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1829160" y="7185960"/>
-        <a:ext cx="9969480" cy="5627880"/>
+        <a:off x="1856160" y="7176960"/>
+        <a:ext cx="9969120" cy="5627520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1591,8 +1582,8 @@
   </sheetPr>
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L18" activeCellId="0" sqref="L18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M18" activeCellId="0" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2148,50 +2139,50 @@
       <c r="J9" s="23" t="n">
         <v>2</v>
       </c>
-      <c r="K9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="N9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="P9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="R9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="S9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="T9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="U9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="V9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="W9" s="25" t="n">
-        <v>0</v>
-      </c>
-      <c r="X9" s="25"/>
+      <c r="K9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="22"/>
     </row>
     <row r="10" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18"/>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -2218,10 +2209,13 @@
       <c r="J10" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="K10" s="27" t="n">
+      <c r="K10" s="26" t="n">
         <v>2</v>
       </c>
       <c r="L10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2317,16 +2311,19 @@
       <c r="H12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I12" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="J12" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="K12" s="29" t="n">
+      <c r="I12" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" s="28" t="n">
         <v>2</v>
       </c>
       <c r="L12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2353,16 +2350,19 @@
       <c r="H13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I13" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="J13" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="K13" s="29" t="n">
+      <c r="I13" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" s="28" t="n">
         <v>2</v>
       </c>
       <c r="L13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="M13" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2439,72 +2439,74 @@
       <c r="A15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="31" t="n">
+      <c r="D15" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="E15" s="31" t="n">
+      <c r="E15" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="F15" s="31" t="n">
+      <c r="F15" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="G15" s="31" t="n">
+      <c r="G15" s="30" t="n">
         <v>3</v>
       </c>
-      <c r="H15" s="32" t="n">
+      <c r="H15" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="I15" s="32" t="n">
+      <c r="I15" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="J15" s="32" t="n">
+      <c r="J15" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="K15" s="33" t="n">
+      <c r="K15" s="32" t="n">
         <v>3</v>
       </c>
-      <c r="L15" s="32" t="n">
+      <c r="L15" s="31" t="n">
         <v>3</v>
       </c>
-      <c r="M15" s="32"/>
-      <c r="N15" s="32"/>
-      <c r="O15" s="32"/>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="32"/>
-      <c r="W15" s="32"/>
+      <c r="M15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="N15" s="31"/>
+      <c r="O15" s="31"/>
+      <c r="P15" s="31"/>
+      <c r="Q15" s="31"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="31"/>
+      <c r="T15" s="31"/>
+      <c r="U15" s="31"/>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18"/>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="26" t="n">
+      <c r="D16" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="E16" s="26" t="n">
+      <c r="E16" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="F16" s="26" t="n">
+      <c r="F16" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="26" t="n">
+      <c r="G16" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="H16" s="35" t="n">
+      <c r="H16" s="34" t="n">
         <v>3</v>
       </c>
       <c r="I16" s="23" t="n">
@@ -2513,45 +2515,47 @@
       <c r="J16" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="K16" s="36" t="n">
+      <c r="K16" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="L16" s="35" t="n">
+      <c r="L16" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
+      <c r="M16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="N16" s="34"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18"/>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="33" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="26" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="35" t="n">
+      <c r="D17" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="34" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="23" t="n">
@@ -2560,117 +2564,119 @@
       <c r="J17" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="K17" s="27" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35"/>
-      <c r="O17" s="35"/>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="35"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
+      <c r="K17" s="26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="34"/>
+      <c r="O17" s="34"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="34"/>
+      <c r="R17" s="34"/>
+      <c r="S17" s="34"/>
+      <c r="T17" s="34"/>
+      <c r="U17" s="34"/>
+      <c r="V17" s="34"/>
+      <c r="W17" s="34"/>
     </row>
     <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="37"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="0" t="n">
         <f aca="false">SUM(D3:D17)</f>
         <v>30</v>
       </c>
-      <c r="E18" s="38" t="n">
+      <c r="E18" s="36" t="n">
         <f aca="false">D18-($D$18/19)</f>
         <v>28.4210526315789</v>
       </c>
-      <c r="F18" s="38" t="n">
+      <c r="F18" s="36" t="n">
         <f aca="false">E18-($D$18/19)</f>
         <v>26.8421052631579</v>
       </c>
-      <c r="G18" s="38" t="n">
+      <c r="G18" s="36" t="n">
         <f aca="false">F18-($D$18/19)</f>
         <v>25.2631578947368</v>
       </c>
-      <c r="H18" s="38" t="n">
+      <c r="H18" s="36" t="n">
         <f aca="false">G18-($D$18/19)</f>
         <v>23.6842105263158</v>
       </c>
-      <c r="I18" s="38" t="n">
+      <c r="I18" s="36" t="n">
         <f aca="false">H18-($D$18/19)</f>
         <v>22.1052631578947</v>
       </c>
-      <c r="J18" s="38" t="n">
+      <c r="J18" s="36" t="n">
         <f aca="false">I18-($D$18/19)</f>
         <v>20.5263157894737</v>
       </c>
-      <c r="K18" s="38" t="n">
+      <c r="K18" s="36" t="n">
         <f aca="false">J18-($D$18/19)</f>
         <v>18.9473684210526</v>
       </c>
-      <c r="L18" s="38" t="n">
+      <c r="L18" s="36" t="n">
         <f aca="false">K18-($D$18/19)</f>
         <v>17.3684210526316</v>
       </c>
-      <c r="M18" s="38" t="n">
+      <c r="M18" s="36" t="n">
         <f aca="false">L18-($D$18/19)</f>
         <v>15.7894736842105</v>
       </c>
-      <c r="N18" s="38" t="n">
+      <c r="N18" s="36" t="n">
         <f aca="false">M18-($D$18/19)</f>
         <v>14.2105263157895</v>
       </c>
-      <c r="O18" s="38" t="n">
+      <c r="O18" s="36" t="n">
         <f aca="false">N18-($D$18/19)</f>
         <v>12.6315789473684</v>
       </c>
-      <c r="P18" s="38" t="n">
+      <c r="P18" s="36" t="n">
         <f aca="false">O18-($D$18/19)</f>
         <v>11.0526315789474</v>
       </c>
-      <c r="Q18" s="38" t="n">
+      <c r="Q18" s="36" t="n">
         <f aca="false">P18-($D$18/19)</f>
         <v>9.47368421052632</v>
       </c>
-      <c r="R18" s="38" t="n">
+      <c r="R18" s="36" t="n">
         <f aca="false">Q18-($D$18/19)</f>
         <v>7.89473684210527</v>
       </c>
-      <c r="S18" s="38" t="n">
+      <c r="S18" s="36" t="n">
         <f aca="false">R18-($D$18/19)</f>
         <v>6.31578947368422</v>
       </c>
-      <c r="T18" s="38" t="n">
+      <c r="T18" s="36" t="n">
         <f aca="false">S18-($D$18/19)</f>
         <v>4.73684210526316</v>
       </c>
-      <c r="U18" s="38" t="n">
+      <c r="U18" s="36" t="n">
         <f aca="false">T18-($D$18/19)</f>
         <v>3.15789473684211</v>
       </c>
-      <c r="V18" s="38" t="n">
+      <c r="V18" s="36" t="n">
         <f aca="false">U18-($D$18/19)</f>
         <v>1.57894736842106</v>
       </c>
-      <c r="W18" s="38" t="n">
+      <c r="W18" s="36" t="n">
         <f aca="false">V18-($D$18/19)</f>
         <v>6.66133814775094E-015</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="30.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="37"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="0" t="n">
         <f aca="false">SUM(D3:D17)</f>
         <v>30</v>
@@ -2709,7 +2715,7 @@
       </c>
       <c r="M19" s="0" t="n">
         <f aca="false">SUM(M3:M17)</f>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N19" s="0" t="n">
         <f aca="false">SUM(N3:N17)</f>

</xml_diff>

<commit_message>
Written few headings of tech and project documentation, updated scrum table to 2015-11-05
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -241,8 +241,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -418,7 +417,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -527,10 +526,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -565,10 +560,6 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -651,7 +642,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1001,22 +992,22 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1029,11 +1020,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="15122242"/>
-        <c:axId val="16494007"/>
+        <c:axId val="13363227"/>
+        <c:axId val="40577217"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="15122242"/>
+        <c:axId val="13363227"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1073,14 +1064,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="16494007"/>
+        <c:crossAx val="40577217"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16494007"/>
+        <c:axId val="40577217"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1130,7 +1121,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="15122242"/>
+        <c:crossAx val="13363227"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1170,15 +1161,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1883160</xdr:colOff>
+      <xdr:colOff>1910160</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>14760</xdr:rowOff>
+      <xdr:rowOff>5760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>877320</xdr:colOff>
+      <xdr:colOff>903960</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>117360</xdr:rowOff>
+      <xdr:rowOff>108000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1186,8 +1177,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1883160" y="7167960"/>
-        <a:ext cx="9968760" cy="5627160"/>
+        <a:off x="1910160" y="7158960"/>
+        <a:ext cx="9968400" cy="5626800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1595,8 +1586,8 @@
   </sheetPr>
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O11" activeCellId="0" sqref="O11"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U17" activeCellId="0" sqref="U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2231,10 +2222,28 @@
       <c r="M10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="N10" s="27" t="n">
+      <c r="N10" s="23" t="n">
         <v>1</v>
       </c>
       <c r="O10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U10" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2330,13 +2339,13 @@
       <c r="H12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I12" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="J12" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="K12" s="29" t="n">
+      <c r="I12" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" s="28" t="n">
         <v>2</v>
       </c>
       <c r="L12" s="0" t="n">
@@ -2345,10 +2354,28 @@
       <c r="M12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N12" s="28" t="n">
+      <c r="N12" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="P12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="R12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="U12" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2375,13 +2402,13 @@
       <c r="H13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I13" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="J13" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="K13" s="29" t="n">
+      <c r="I13" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" s="28" t="n">
         <v>2</v>
       </c>
       <c r="L13" s="0" t="n">
@@ -2390,10 +2417,28 @@
       <c r="M13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="N13" s="28" t="n">
+      <c r="N13" s="27" t="n">
         <v>2</v>
       </c>
       <c r="O13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="P13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="R13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="S13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="T13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="U13" s="0" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2470,60 +2515,72 @@
       <c r="A15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="31" t="n">
-        <v>3</v>
-      </c>
-      <c r="E15" s="31" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" s="31" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" s="31" t="n">
-        <v>3</v>
-      </c>
-      <c r="H15" s="32" t="n">
-        <v>3</v>
-      </c>
-      <c r="I15" s="32" t="n">
-        <v>3</v>
-      </c>
-      <c r="J15" s="32" t="n">
-        <v>3</v>
-      </c>
-      <c r="K15" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="L15" s="32" t="n">
-        <v>3</v>
-      </c>
-      <c r="M15" s="32" t="n">
-        <v>3</v>
-      </c>
-      <c r="N15" s="32" t="n">
-        <v>3</v>
-      </c>
-      <c r="O15" s="32" t="n">
-        <v>3</v>
-      </c>
-      <c r="P15" s="32"/>
-      <c r="Q15" s="32"/>
-      <c r="R15" s="32"/>
-      <c r="S15" s="32"/>
-      <c r="T15" s="32"/>
-      <c r="U15" s="32"/>
-      <c r="V15" s="32"/>
-      <c r="W15" s="32"/>
+      <c r="D15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" s="32" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="M15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="N15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="O15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="P15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="R15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="S15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="T15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="U15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="V15" s="31"/>
+      <c r="W15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="18"/>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="33" t="s">
         <v>44</v>
       </c>
       <c r="C16" s="25" t="s">
@@ -2541,7 +2598,7 @@
       <c r="G16" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="H16" s="35" t="n">
+      <c r="H16" s="34" t="n">
         <v>3</v>
       </c>
       <c r="I16" s="23" t="n">
@@ -2553,30 +2610,42 @@
       <c r="K16" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="L16" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="M16" s="35" t="n">
+      <c r="L16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="M16" s="34" t="n">
         <v>3</v>
       </c>
       <c r="N16" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="O16" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
+      <c r="O16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="P16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="R16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="S16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="T16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="U16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="V16" s="34"/>
+      <c r="W16" s="34"/>
     </row>
     <row r="17" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18"/>
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="35" t="s">
         <v>45</v>
       </c>
       <c r="C17" s="25" t="s">
@@ -2594,7 +2663,7 @@
       <c r="G17" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="H17" s="35" t="n">
+      <c r="H17" s="34" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="23" t="n">
@@ -2606,13 +2675,13 @@
       <c r="K17" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="L17" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" s="35" t="n">
-        <v>1</v>
-      </c>
-      <c r="N17" s="37" t="n">
+      <c r="L17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="N17" s="22" t="n">
         <v>0</v>
       </c>
       <c r="O17" s="20" t="n">
@@ -2644,98 +2713,98 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="38" t="s">
+      <c r="A18" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="0" t="n">
         <f aca="false">SUM(D3:D17)</f>
         <v>30</v>
       </c>
-      <c r="E18" s="39" t="n">
+      <c r="E18" s="37" t="n">
         <f aca="false">D18-($D$18/19)</f>
         <v>28.4210526315789</v>
       </c>
-      <c r="F18" s="39" t="n">
+      <c r="F18" s="37" t="n">
         <f aca="false">E18-($D$18/19)</f>
         <v>26.8421052631579</v>
       </c>
-      <c r="G18" s="39" t="n">
+      <c r="G18" s="37" t="n">
         <f aca="false">F18-($D$18/19)</f>
         <v>25.2631578947368</v>
       </c>
-      <c r="H18" s="39" t="n">
+      <c r="H18" s="37" t="n">
         <f aca="false">G18-($D$18/19)</f>
         <v>23.6842105263158</v>
       </c>
-      <c r="I18" s="39" t="n">
+      <c r="I18" s="37" t="n">
         <f aca="false">H18-($D$18/19)</f>
         <v>22.1052631578947</v>
       </c>
-      <c r="J18" s="39" t="n">
+      <c r="J18" s="37" t="n">
         <f aca="false">I18-($D$18/19)</f>
         <v>20.5263157894737</v>
       </c>
-      <c r="K18" s="39" t="n">
+      <c r="K18" s="37" t="n">
         <f aca="false">J18-($D$18/19)</f>
         <v>18.9473684210526</v>
       </c>
-      <c r="L18" s="39" t="n">
+      <c r="L18" s="37" t="n">
         <f aca="false">K18-($D$18/19)</f>
         <v>17.3684210526316</v>
       </c>
-      <c r="M18" s="39" t="n">
+      <c r="M18" s="37" t="n">
         <f aca="false">L18-($D$18/19)</f>
         <v>15.7894736842105</v>
       </c>
-      <c r="N18" s="39" t="n">
+      <c r="N18" s="37" t="n">
         <f aca="false">M18-($D$18/19)</f>
         <v>14.2105263157895</v>
       </c>
-      <c r="O18" s="39" t="n">
+      <c r="O18" s="37" t="n">
         <f aca="false">N18-($D$18/19)</f>
         <v>12.6315789473684</v>
       </c>
-      <c r="P18" s="39" t="n">
+      <c r="P18" s="37" t="n">
         <f aca="false">O18-($D$18/19)</f>
         <v>11.0526315789474</v>
       </c>
-      <c r="Q18" s="39" t="n">
+      <c r="Q18" s="37" t="n">
         <f aca="false">P18-($D$18/19)</f>
         <v>9.47368421052632</v>
       </c>
-      <c r="R18" s="39" t="n">
+      <c r="R18" s="37" t="n">
         <f aca="false">Q18-($D$18/19)</f>
         <v>7.89473684210527</v>
       </c>
-      <c r="S18" s="39" t="n">
+      <c r="S18" s="37" t="n">
         <f aca="false">R18-($D$18/19)</f>
         <v>6.31578947368422</v>
       </c>
-      <c r="T18" s="39" t="n">
+      <c r="T18" s="37" t="n">
         <f aca="false">S18-($D$18/19)</f>
         <v>4.73684210526316</v>
       </c>
-      <c r="U18" s="39" t="n">
+      <c r="U18" s="37" t="n">
         <f aca="false">T18-($D$18/19)</f>
         <v>3.15789473684211</v>
       </c>
-      <c r="V18" s="39" t="n">
+      <c r="V18" s="37" t="n">
         <f aca="false">U18-($D$18/19)</f>
         <v>1.57894736842106</v>
       </c>
-      <c r="W18" s="39" t="n">
+      <c r="W18" s="37" t="n">
         <f aca="false">V18-($D$18/19)</f>
         <v>6.66133814775094E-015</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="30.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="0" t="n">
         <f aca="false">SUM(D3:D17)</f>
         <v>30</v>
@@ -2786,27 +2855,27 @@
       </c>
       <c r="P19" s="0" t="n">
         <f aca="false">SUM(P3:P17)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Q19" s="0" t="n">
         <f aca="false">SUM(Q3:Q17)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="R19" s="0" t="n">
         <f aca="false">SUM(R3:R17)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="S19" s="0" t="n">
         <f aca="false">SUM(S3:S17)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="T19" s="0" t="n">
         <f aca="false">SUM(T3:T17)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U19" s="0" t="n">
         <f aca="false">SUM(U3:U17)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="V19" s="0" t="n">
         <f aca="false">SUM(V3:V17)</f>

</xml_diff>

<commit_message>
Refactored code to use two service calls on registration, added session on successful login and toString methods to model classes
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -417,7 +417,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -518,7 +518,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -551,6 +551,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1004,10 +1008,10 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1020,11 +1024,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="13363227"/>
-        <c:axId val="40577217"/>
+        <c:axId val="50736480"/>
+        <c:axId val="99679485"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="13363227"/>
+        <c:axId val="50736480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,14 +1068,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="40577217"/>
+        <c:crossAx val="99679485"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40577217"/>
+        <c:axId val="99679485"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1121,7 +1125,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="13363227"/>
+        <c:crossAx val="50736480"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1161,15 +1165,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1910160</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>5760</xdr:rowOff>
+      <xdr:colOff>1937160</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>187200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>903960</xdr:colOff>
+      <xdr:colOff>930600</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>108000</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1177,8 +1181,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1910160" y="7158960"/>
-        <a:ext cx="9968400" cy="5626800"/>
+        <a:off x="1937160" y="7149960"/>
+        <a:ext cx="9968040" cy="5626440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1199,7 +1203,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="W10 D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1478,7 +1482,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="W10 E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1587,7 +1591,7 @@
   <dimension ref="A1:X19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U17" activeCellId="0" sqref="U17"/>
+      <selection pane="topLeft" activeCell="W10" activeCellId="0" sqref="W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2240,11 +2244,17 @@
       <c r="S10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="T10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="U10" s="0" t="n">
-        <v>1</v>
+      <c r="T10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2583,22 +2593,22 @@
       <c r="B16" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="25" t="n">
-        <v>3</v>
-      </c>
-      <c r="E16" s="25" t="n">
-        <v>3</v>
-      </c>
-      <c r="F16" s="25" t="n">
-        <v>3</v>
-      </c>
-      <c r="G16" s="25" t="n">
-        <v>3</v>
-      </c>
-      <c r="H16" s="34" t="n">
+      <c r="D16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="35" t="n">
         <v>3</v>
       </c>
       <c r="I16" s="23" t="n">
@@ -2610,60 +2620,60 @@
       <c r="K16" s="26" t="n">
         <v>3</v>
       </c>
-      <c r="L16" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="M16" s="34" t="n">
+      <c r="L16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="M16" s="35" t="n">
         <v>3</v>
       </c>
       <c r="N16" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="O16" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="P16" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q16" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="R16" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="S16" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="T16" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="U16" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="V16" s="34"/>
-      <c r="W16" s="34"/>
+      <c r="O16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="P16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="R16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="S16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="T16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="U16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="V16" s="35"/>
+      <c r="W16" s="35"/>
     </row>
     <row r="17" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="18"/>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="34" t="n">
+      <c r="D17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="35" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="23" t="n">
@@ -2675,10 +2685,10 @@
       <c r="K17" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="L17" s="34" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" s="34" t="n">
+      <c r="L17" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="35" t="n">
         <v>1</v>
       </c>
       <c r="N17" s="22" t="n">
@@ -2713,98 +2723,98 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
       <c r="D18" s="0" t="n">
         <f aca="false">SUM(D3:D17)</f>
         <v>30</v>
       </c>
-      <c r="E18" s="37" t="n">
+      <c r="E18" s="38" t="n">
         <f aca="false">D18-($D$18/19)</f>
         <v>28.4210526315789</v>
       </c>
-      <c r="F18" s="37" t="n">
+      <c r="F18" s="38" t="n">
         <f aca="false">E18-($D$18/19)</f>
         <v>26.8421052631579</v>
       </c>
-      <c r="G18" s="37" t="n">
+      <c r="G18" s="38" t="n">
         <f aca="false">F18-($D$18/19)</f>
         <v>25.2631578947368</v>
       </c>
-      <c r="H18" s="37" t="n">
+      <c r="H18" s="38" t="n">
         <f aca="false">G18-($D$18/19)</f>
         <v>23.6842105263158</v>
       </c>
-      <c r="I18" s="37" t="n">
+      <c r="I18" s="38" t="n">
         <f aca="false">H18-($D$18/19)</f>
         <v>22.1052631578947</v>
       </c>
-      <c r="J18" s="37" t="n">
+      <c r="J18" s="38" t="n">
         <f aca="false">I18-($D$18/19)</f>
         <v>20.5263157894737</v>
       </c>
-      <c r="K18" s="37" t="n">
+      <c r="K18" s="38" t="n">
         <f aca="false">J18-($D$18/19)</f>
         <v>18.9473684210526</v>
       </c>
-      <c r="L18" s="37" t="n">
+      <c r="L18" s="38" t="n">
         <f aca="false">K18-($D$18/19)</f>
         <v>17.3684210526316</v>
       </c>
-      <c r="M18" s="37" t="n">
+      <c r="M18" s="38" t="n">
         <f aca="false">L18-($D$18/19)</f>
         <v>15.7894736842105</v>
       </c>
-      <c r="N18" s="37" t="n">
+      <c r="N18" s="38" t="n">
         <f aca="false">M18-($D$18/19)</f>
         <v>14.2105263157895</v>
       </c>
-      <c r="O18" s="37" t="n">
+      <c r="O18" s="38" t="n">
         <f aca="false">N18-($D$18/19)</f>
         <v>12.6315789473684</v>
       </c>
-      <c r="P18" s="37" t="n">
+      <c r="P18" s="38" t="n">
         <f aca="false">O18-($D$18/19)</f>
         <v>11.0526315789474</v>
       </c>
-      <c r="Q18" s="37" t="n">
+      <c r="Q18" s="38" t="n">
         <f aca="false">P18-($D$18/19)</f>
         <v>9.47368421052632</v>
       </c>
-      <c r="R18" s="37" t="n">
+      <c r="R18" s="38" t="n">
         <f aca="false">Q18-($D$18/19)</f>
         <v>7.89473684210527</v>
       </c>
-      <c r="S18" s="37" t="n">
+      <c r="S18" s="38" t="n">
         <f aca="false">R18-($D$18/19)</f>
         <v>6.31578947368422</v>
       </c>
-      <c r="T18" s="37" t="n">
+      <c r="T18" s="38" t="n">
         <f aca="false">S18-($D$18/19)</f>
         <v>4.73684210526316</v>
       </c>
-      <c r="U18" s="37" t="n">
+      <c r="U18" s="38" t="n">
         <f aca="false">T18-($D$18/19)</f>
         <v>3.15789473684211</v>
       </c>
-      <c r="V18" s="37" t="n">
+      <c r="V18" s="38" t="n">
         <f aca="false">U18-($D$18/19)</f>
         <v>1.57894736842106</v>
       </c>
-      <c r="W18" s="37" t="n">
+      <c r="W18" s="38" t="n">
         <f aca="false">V18-($D$18/19)</f>
         <v>6.66133814775094E-015</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="30.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
       <c r="D19" s="0" t="n">
         <f aca="false">SUM(D3:D17)</f>
         <v>30</v>
@@ -2871,11 +2881,11 @@
       </c>
       <c r="T19" s="0" t="n">
         <f aca="false">SUM(T3:T17)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U19" s="0" t="n">
         <f aca="false">SUM(U3:U17)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="V19" s="0" t="n">
         <f aca="false">SUM(V3:V17)</f>

</xml_diff>

<commit_message>
Added some text to project documentation
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -1011,7 +1011,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>0</c:v>
@@ -1024,11 +1024,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="50736480"/>
-        <c:axId val="99679485"/>
+        <c:axId val="87394286"/>
+        <c:axId val="44425196"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="50736480"/>
+        <c:axId val="87394286"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,14 +1068,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="99679485"/>
+        <c:crossAx val="44425196"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="99679485"/>
+        <c:axId val="44425196"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1125,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="50736480"/>
+        <c:crossAx val="87394286"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1165,15 +1165,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1937160</xdr:colOff>
+      <xdr:colOff>1964160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>187200</xdr:rowOff>
+      <xdr:rowOff>178200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>930600</xdr:colOff>
+      <xdr:colOff>957240</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>98640</xdr:rowOff>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1181,8 +1181,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1937160" y="7149960"/>
-        <a:ext cx="9968040" cy="5626440"/>
+        <a:off x="1964160" y="7140960"/>
+        <a:ext cx="9967680" cy="5626080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1203,7 +1203,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="1" sqref="W10 D4"/>
+      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1482,7 +1482,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="W10 E13"/>
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1590,8 +1590,8 @@
   </sheetPr>
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W10" activeCellId="0" sqref="W10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V13" activeCellId="0" sqref="V13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2328,7 +2328,7 @@
     </row>
     <row r="12" customFormat="false" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="18"/>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="19" t="s">
         <v>39</v>
       </c>
       <c r="C12" s="6" t="s">
@@ -2385,8 +2385,14 @@
       <c r="T12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="U12" s="0" t="n">
-        <v>1</v>
+      <c r="U12" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2885,7 +2891,7 @@
       </c>
       <c r="U19" s="0" t="n">
         <f aca="false">SUM(U3:U17)</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V19" s="0" t="n">
         <f aca="false">SUM(V3:V17)</f>

</xml_diff>

<commit_message>
added readObject implementation to ServiceParams
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -1024,11 +1024,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87394286"/>
-        <c:axId val="44425196"/>
+        <c:axId val="79000826"/>
+        <c:axId val="68460248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87394286"/>
+        <c:axId val="79000826"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1068,14 +1068,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44425196"/>
+        <c:crossAx val="68460248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="44425196"/>
+        <c:axId val="68460248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1125,7 +1125,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="87394286"/>
+        <c:crossAx val="79000826"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1165,15 +1165,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1964160</xdr:colOff>
+      <xdr:colOff>1991160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>178200</xdr:rowOff>
+      <xdr:rowOff>169200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>957240</xdr:colOff>
+      <xdr:colOff>983880</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>89280</xdr:rowOff>
+      <xdr:rowOff>79920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1181,8 +1181,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1964160" y="7140960"/>
-        <a:ext cx="9967680" cy="5626080"/>
+        <a:off x="1991160" y="7131960"/>
+        <a:ext cx="9967320" cy="5625720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1590,8 +1590,8 @@
   </sheetPr>
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="V13" activeCellId="0" sqref="V13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I35" activeCellId="0" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
refactored for modularity, updated scrum tables
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="61">
   <si>
     <t>New estimates of effort remaining as of sprint</t>
   </si>
@@ -177,6 +177,12 @@
   </si>
   <si>
     <t>izraditi web servis za kreiranje grupe</t>
+  </si>
+  <si>
+    <t>izraditi logo aplikacije</t>
+  </si>
+  <si>
+    <t>refaktorirati kod za modularnost</t>
   </si>
   <si>
     <t>izraditi početni activity sa fragmentima</t>
@@ -206,7 +212,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -275,8 +281,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -287,12 +292,8 @@
       <family val="2"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -725,7 +726,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1103,11 +1104,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="27014950"/>
-        <c:axId val="23366421"/>
+        <c:axId val="70625855"/>
+        <c:axId val="21423934"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="27014950"/>
+        <c:axId val="70625855"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1147,14 +1148,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23366421"/>
+        <c:crossAx val="21423934"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23366421"/>
+        <c:axId val="21423934"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1204,7 +1205,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="27014950"/>
+        <c:crossAx val="70625855"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1239,7 +1240,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1253,7 +1254,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Burndown chart</a:t>
@@ -1293,7 +1294,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1372,7 +1373,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2 backlog'!$D$13:$W$13</c:f>
+              <c:f>'Sprint 2 backlog'!$D$15:$W$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1466,7 +1467,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1545,7 +1546,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2 backlog'!$D$14:$W$14</c:f>
+              <c:f>'Sprint 2 backlog'!$D$16:$W$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1553,7 +1554,7 @@
                   <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1614,11 +1615,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84041667"/>
-        <c:axId val="84307201"/>
+        <c:axId val="29838863"/>
+        <c:axId val="8859545"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84041667"/>
+        <c:axId val="29838863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1634,14 +1635,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84307201"/>
+        <c:crossAx val="8859545"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84307201"/>
+        <c:axId val="8859545"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1666,8 +1667,8 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84041667"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="29838863"/>
+        <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1706,15 +1707,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2018160</xdr:colOff>
+      <xdr:colOff>2045160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>151200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1010520</xdr:colOff>
+      <xdr:colOff>1037160</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>70560</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1722,8 +1723,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2018160" y="7210440"/>
-        <a:ext cx="9966960" cy="5625360"/>
+        <a:off x="2045160" y="7201440"/>
+        <a:ext cx="9966600" cy="5625000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1741,15 +1742,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2380320</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>381240</xdr:rowOff>
+      <xdr:colOff>2407320</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>372600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>475200</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>128160</xdr:rowOff>
+      <xdr:colOff>501840</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>119160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1757,8 +1758,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2380320" y="6228720"/>
-        <a:ext cx="9046080" cy="4866840"/>
+        <a:off x="2407320" y="7129440"/>
+        <a:ext cx="9045720" cy="4307760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1778,7 +1779,7 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -2083,7 +2084,7 @@
   </sheetPr>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -2192,7 +2193,7 @@
   </sheetPr>
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="W9" activeCellId="0" sqref="W9"/>
     </sheetView>
   </sheetViews>
@@ -3544,8 +3545,8 @@
   </sheetPr>
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X2" activeCellId="0" sqref="X2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3669,7 +3670,9 @@
       <c r="D3" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="21"/>
+      <c r="E3" s="23" t="n">
+        <v>3</v>
+      </c>
       <c r="F3" s="21"/>
       <c r="G3" s="21"/>
       <c r="H3" s="22"/>
@@ -3700,7 +3703,9 @@
       <c r="D4" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E4" s="21"/>
+      <c r="E4" s="23" t="n">
+        <v>2</v>
+      </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
@@ -3729,9 +3734,11 @@
         <v>29</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="E5" s="23" t="n">
+        <v>1</v>
+      </c>
       <c r="F5" s="23"/>
       <c r="G5" s="21"/>
       <c r="H5" s="22"/>
@@ -3762,7 +3769,9 @@
       <c r="D6" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="23"/>
+      <c r="E6" s="23" t="n">
+        <v>3</v>
+      </c>
       <c r="F6" s="23"/>
       <c r="G6" s="6"/>
       <c r="I6" s="24"/>
@@ -3792,7 +3801,9 @@
       <c r="D7" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="23" t="n">
+        <v>4</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="I7" s="24"/>
@@ -3817,15 +3828,17 @@
         <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>5</v>
-      </c>
-      <c r="E8" s="6"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="23" t="n">
+        <v>1</v>
+      </c>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
-      <c r="I8" s="25"/>
+      <c r="I8" s="24"/>
       <c r="J8" s="24"/>
       <c r="K8" s="24"/>
       <c r="L8" s="24"/>
@@ -3843,313 +3856,420 @@
     </row>
     <row r="9" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20"/>
-      <c r="B9" s="43" t="s">
-        <v>55</v>
+      <c r="B9" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
+        <v>1</v>
+      </c>
+      <c r="E9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="44" t="s">
+      <c r="A10" s="20"/>
+      <c r="B10" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C10" s="33" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="35"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-      <c r="U10" s="34"/>
-      <c r="V10" s="36"/>
-      <c r="W10" s="36"/>
+      <c r="D10" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" s="23" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
+      <c r="O10" s="24"/>
+      <c r="P10" s="24"/>
+      <c r="Q10" s="24"/>
+      <c r="R10" s="24"/>
+      <c r="S10" s="24"/>
+      <c r="T10" s="24"/>
+      <c r="U10" s="24"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="37.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="39"/>
+      <c r="C11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
       <c r="I11" s="25"/>
       <c r="J11" s="25"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="40"/>
-      <c r="W11" s="40"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
     </row>
     <row r="12" customFormat="false" ht="42.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="20"/>
-      <c r="B12" s="45" t="s">
+      <c r="A12" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="33" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="33" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="34"/>
+      <c r="R12" s="34"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+      <c r="U12" s="34"/>
+      <c r="V12" s="36"/>
+      <c r="W12" s="36"/>
+    </row>
+    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20"/>
+      <c r="B13" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="39"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="39"/>
+      <c r="P13" s="39"/>
+      <c r="Q13" s="39"/>
+      <c r="R13" s="39"/>
+      <c r="S13" s="39"/>
+      <c r="T13" s="39"/>
+      <c r="U13" s="39"/>
+      <c r="V13" s="40"/>
+      <c r="W13" s="40"/>
+    </row>
+    <row r="14" customFormat="false" ht="33.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="20"/>
+      <c r="B14" s="45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="22"/>
-      <c r="S12" s="22"/>
-      <c r="T12" s="22"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="22"/>
-      <c r="W12" s="22"/>
-    </row>
-    <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41" t="s">
+      <c r="D14" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="24"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="22"/>
+      <c r="U14" s="22"/>
+      <c r="V14" s="22"/>
+      <c r="W14" s="22"/>
+    </row>
+    <row r="15" customFormat="false" ht="36.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="0" t="n">
-        <f aca="false">SUM(D3:D12)</f>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="0" t="n">
+        <f aca="false">SUM(D3:D14)</f>
         <v>27</v>
       </c>
-      <c r="E13" s="42" t="n">
-        <f aca="false">D13-($D$13/19)</f>
+      <c r="E15" s="42" t="n">
+        <f aca="false">D15-($D$15/19)</f>
         <v>25.5789473684211</v>
       </c>
-      <c r="F13" s="42" t="n">
-        <f aca="false">E13-($D$13/19)</f>
+      <c r="F15" s="42" t="n">
+        <f aca="false">E15-($D$15/19)</f>
         <v>24.1578947368421</v>
       </c>
-      <c r="G13" s="42" t="n">
-        <f aca="false">F13-($D$13/19)</f>
+      <c r="G15" s="42" t="n">
+        <f aca="false">F15-($D$15/19)</f>
         <v>22.7368421052632</v>
       </c>
-      <c r="H13" s="42" t="n">
-        <f aca="false">G13-($D$13/19)</f>
+      <c r="H15" s="42" t="n">
+        <f aca="false">G15-($D$15/19)</f>
         <v>21.3157894736842</v>
       </c>
-      <c r="I13" s="42" t="n">
-        <f aca="false">H13-($D$13/19)</f>
+      <c r="I15" s="42" t="n">
+        <f aca="false">H15-($D$15/19)</f>
         <v>19.8947368421053</v>
       </c>
-      <c r="J13" s="42" t="n">
-        <f aca="false">I13-($D$13/19)</f>
+      <c r="J15" s="42" t="n">
+        <f aca="false">I15-($D$15/19)</f>
         <v>18.4736842105263</v>
       </c>
-      <c r="K13" s="42" t="n">
-        <f aca="false">J13-($D$13/19)</f>
+      <c r="K15" s="42" t="n">
+        <f aca="false">J15-($D$15/19)</f>
         <v>17.0526315789474</v>
       </c>
-      <c r="L13" s="42" t="n">
-        <f aca="false">K13-($D$13/19)</f>
+      <c r="L15" s="42" t="n">
+        <f aca="false">K15-($D$15/19)</f>
         <v>15.6315789473684</v>
       </c>
-      <c r="M13" s="42" t="n">
-        <f aca="false">L13-($D$13/19)</f>
+      <c r="M15" s="42" t="n">
+        <f aca="false">L15-($D$15/19)</f>
         <v>14.2105263157895</v>
       </c>
-      <c r="N13" s="42" t="n">
-        <f aca="false">M13-($D$13/19)</f>
+      <c r="N15" s="42" t="n">
+        <f aca="false">M15-($D$15/19)</f>
         <v>12.7894736842105</v>
       </c>
-      <c r="O13" s="42" t="n">
-        <f aca="false">N13-($D$13/19)</f>
+      <c r="O15" s="42" t="n">
+        <f aca="false">N15-($D$15/19)</f>
         <v>11.3684210526316</v>
       </c>
-      <c r="P13" s="42" t="n">
-        <f aca="false">O13-($D$13/19)</f>
+      <c r="P15" s="42" t="n">
+        <f aca="false">O15-($D$15/19)</f>
         <v>9.94736842105263</v>
       </c>
-      <c r="Q13" s="42" t="n">
-        <f aca="false">P13-($D$13/19)</f>
+      <c r="Q15" s="42" t="n">
+        <f aca="false">P15-($D$15/19)</f>
         <v>8.52631578947368</v>
       </c>
-      <c r="R13" s="42" t="n">
-        <f aca="false">Q13-($D$13/19)</f>
+      <c r="R15" s="42" t="n">
+        <f aca="false">Q15-($D$15/19)</f>
         <v>7.10526315789473</v>
       </c>
-      <c r="S13" s="42" t="n">
-        <f aca="false">R13-($D$13/19)</f>
+      <c r="S15" s="42" t="n">
+        <f aca="false">R15-($D$15/19)</f>
         <v>5.68421052631578</v>
       </c>
-      <c r="T13" s="42" t="n">
-        <f aca="false">S13-($D$13/19)</f>
+      <c r="T15" s="42" t="n">
+        <f aca="false">S15-($D$15/19)</f>
         <v>4.26315789473684</v>
       </c>
-      <c r="U13" s="42" t="n">
-        <f aca="false">T13-($D$13/19)</f>
+      <c r="U15" s="42" t="n">
+        <f aca="false">T15-($D$15/19)</f>
         <v>2.84210526315789</v>
       </c>
-      <c r="V13" s="42" t="n">
-        <f aca="false">U13-($D$13/19)</f>
+      <c r="V15" s="42" t="n">
+        <f aca="false">U15-($D$15/19)</f>
         <v>1.42105263157894</v>
       </c>
-      <c r="W13" s="42" t="n">
-        <f aca="false">V13-($D$13/19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="33.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41" t="s">
+      <c r="W15" s="42" t="n">
+        <f aca="false">V15-($D$15/19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="0" t="n">
-        <f aca="false">SUM(D3:D12)</f>
+      <c r="B16" s="41"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="0" t="n">
+        <f aca="false">SUM(D3:D14)</f>
         <v>27</v>
       </c>
-      <c r="E14" s="0" t="n">
-        <f aca="false">SUM(E3:E12)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <f aca="false">SUM(F3:F12)</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <f aca="false">SUM(G3:G12)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">SUM(H3:H12)</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="0" t="n">
-        <f aca="false">SUM(I3:I12)</f>
-        <v>0</v>
-      </c>
-      <c r="J14" s="0" t="n">
-        <f aca="false">SUM(J3:J12)</f>
-        <v>0</v>
-      </c>
-      <c r="K14" s="0" t="n">
-        <f aca="false">SUM(K3:K12)</f>
-        <v>0</v>
-      </c>
-      <c r="L14" s="0" t="n">
-        <f aca="false">SUM(L3:L12)</f>
-        <v>0</v>
-      </c>
-      <c r="M14" s="0" t="n">
-        <f aca="false">SUM(M3:M12)</f>
-        <v>0</v>
-      </c>
-      <c r="N14" s="0" t="n">
-        <f aca="false">SUM(N3:N12)</f>
-        <v>0</v>
-      </c>
-      <c r="O14" s="0" t="n">
-        <f aca="false">SUM(O3:O12)</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="0" t="n">
-        <f aca="false">SUM(P3:P12)</f>
-        <v>0</v>
-      </c>
-      <c r="Q14" s="0" t="n">
-        <f aca="false">SUM(Q3:Q12)</f>
-        <v>0</v>
-      </c>
-      <c r="R14" s="0" t="n">
-        <f aca="false">SUM(R3:R12)</f>
-        <v>0</v>
-      </c>
-      <c r="S14" s="0" t="n">
-        <f aca="false">SUM(S3:S12)</f>
-        <v>0</v>
-      </c>
-      <c r="T14" s="0" t="n">
-        <f aca="false">SUM(T3:T12)</f>
-        <v>0</v>
-      </c>
-      <c r="U14" s="0" t="n">
-        <f aca="false">SUM(U3:U12)</f>
-        <v>0</v>
-      </c>
-      <c r="V14" s="0" t="n">
-        <f aca="false">SUM(V3:V12)</f>
-        <v>0</v>
-      </c>
-      <c r="W14" s="0" t="n">
-        <f aca="false">SUM(W3:W12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="36.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="E16" s="0" t="n">
+        <f aca="false">SUM(E3:E14)</f>
+        <v>26</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <f aca="false">SUM(F3:F14)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <f aca="false">SUM(G3:G14)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <f aca="false">SUM(H3:H14)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <f aca="false">SUM(I3:I14)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="0" t="n">
+        <f aca="false">SUM(J3:J14)</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <f aca="false">SUM(K3:K14)</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <f aca="false">SUM(L3:L14)</f>
+        <v>0</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <f aca="false">SUM(M3:M14)</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="0" t="n">
+        <f aca="false">SUM(N3:N14)</f>
+        <v>0</v>
+      </c>
+      <c r="O16" s="0" t="n">
+        <f aca="false">SUM(O3:O14)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="0" t="n">
+        <f aca="false">SUM(P3:P14)</f>
+        <v>0</v>
+      </c>
+      <c r="Q16" s="0" t="n">
+        <f aca="false">SUM(Q3:Q14)</f>
+        <v>0</v>
+      </c>
+      <c r="R16" s="0" t="n">
+        <f aca="false">SUM(R3:R14)</f>
+        <v>0</v>
+      </c>
+      <c r="S16" s="0" t="n">
+        <f aca="false">SUM(S3:S14)</f>
+        <v>0</v>
+      </c>
+      <c r="T16" s="0" t="n">
+        <f aca="false">SUM(T3:T14)</f>
+        <v>0</v>
+      </c>
+      <c r="U16" s="0" t="n">
+        <f aca="false">SUM(U3:U14)</f>
+        <v>0</v>
+      </c>
+      <c r="V16" s="0" t="n">
+        <f aca="false">SUM(V3:V14)</f>
+        <v>0</v>
+      </c>
+      <c r="W16" s="0" t="n">
+        <f aca="false">SUM(W3:W14)</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="17" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="E1:W1"/>
-    <mergeCell ref="A3:A9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="A12:A14"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A16:C16"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
napravljena ikona, fragmenti, history i navigacija
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -469,7 +469,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="43">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -642,18 +642,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -726,7 +714,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1104,11 +1092,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74379486"/>
-        <c:axId val="11857149"/>
+        <c:axId val="93650457"/>
+        <c:axId val="26879203"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74379486"/>
+        <c:axId val="93650457"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,14 +1136,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="11857149"/>
+        <c:crossAx val="26879203"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11857149"/>
+        <c:axId val="26879203"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,7 +1193,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="74379486"/>
+        <c:crossAx val="93650457"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1240,7 +1228,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1294,7 +1282,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1467,7 +1455,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="4"/>
+            <c:size val="2"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1615,11 +1603,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77309141"/>
-        <c:axId val="19527324"/>
+        <c:axId val="88571738"/>
+        <c:axId val="53682345"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77309141"/>
+        <c:axId val="88571738"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1635,14 +1623,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="19527324"/>
+        <c:crossAx val="53682345"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19527324"/>
+        <c:axId val="53682345"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1667,7 +1655,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="77309141"/>
+        <c:crossAx val="88571738"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1707,15 +1695,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2099160</xdr:colOff>
+      <xdr:colOff>2153160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1090440</xdr:colOff>
+      <xdr:colOff>1143720</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>42480</xdr:rowOff>
+      <xdr:rowOff>23760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1723,8 +1711,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2099160" y="7183440"/>
-        <a:ext cx="9965880" cy="5624280"/>
+        <a:off x="2153160" y="7165440"/>
+        <a:ext cx="9965160" cy="5623560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1741,16 +1729,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2461320</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>354600</xdr:rowOff>
+      <xdr:rowOff>317520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>555120</xdr:colOff>
+      <xdr:colOff>608400</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1758,8 +1746,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2461320" y="7111440"/>
-        <a:ext cx="9045000" cy="4307040"/>
+        <a:off x="2515320" y="7093440"/>
+        <a:ext cx="9044280" cy="4306320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1779,8 +1767,8 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1832,7 +1820,7 @@
       </c>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -1848,12 +1836,14 @@
       <c r="E3" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F3" s="7"/>
+      <c r="F3" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1869,12 +1859,14 @@
       <c r="E4" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>7</v>
       </c>
@@ -1890,12 +1882,14 @@
       <c r="E5" s="7" t="n">
         <v>21</v>
       </c>
-      <c r="F5" s="7"/>
+      <c r="F5" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -1911,12 +1905,14 @@
       <c r="E6" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="F6" s="7"/>
+      <c r="F6" s="7" t="n">
+        <v>0</v>
+      </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -1932,12 +1928,14 @@
       <c r="E7" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7" t="n">
+        <v>11</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="6"/>
     </row>
-    <row r="8" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -1953,12 +1951,14 @@
       <c r="E8" s="7" t="n">
         <v>32</v>
       </c>
-      <c r="F8" s="7"/>
+      <c r="F8" s="7" t="n">
+        <v>32</v>
+      </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
       <c r="I8" s="6"/>
     </row>
-    <row r="9" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -1974,7 +1974,9 @@
       <c r="E9" s="7" t="n">
         <v>22</v>
       </c>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="n">
+        <v>22</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="6"/>
@@ -1995,12 +1997,14 @@
       <c r="E10" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="8" t="n">
+        <v>6</v>
+      </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -2016,12 +2020,14 @@
       <c r="E11" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="n">
+        <v>8</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>14</v>
       </c>
@@ -2037,12 +2043,14 @@
       <c r="E12" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="F12" s="7"/>
+      <c r="F12" s="7" t="n">
+        <v>16</v>
+      </c>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
       <c r="I12" s="6"/>
     </row>
-    <row r="13" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -2058,7 +2066,9 @@
       <c r="E13" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="7" t="n">
+        <v>4</v>
+      </c>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
       <c r="I13" s="6"/>
@@ -3545,8 +3555,8 @@
   </sheetPr>
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -3661,7 +3671,7 @@
       <c r="A3" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -3673,55 +3683,55 @@
       <c r="E3" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="F3" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" s="21" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="I3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="K3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="L3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="M3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="N3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="O3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="P3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="R3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="S3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="T3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="U3" s="22" t="n">
-        <v>3</v>
-      </c>
-      <c r="V3" s="22" t="n">
+      <c r="F3" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="H3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="N3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="O3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="P3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="R3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="S3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="T3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="U3" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="V3" s="29" t="n">
         <v>1</v>
       </c>
       <c r="W3" s="22" t="n">
@@ -3730,7 +3740,7 @@
     </row>
     <row r="4" customFormat="false" ht="27.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20"/>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="21" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -3797,9 +3807,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20"/>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -3814,52 +3824,52 @@
       <c r="F5" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="G5" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="R5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="S5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" s="22" t="n">
-        <v>1</v>
-      </c>
-      <c r="V5" s="22" t="n">
+      <c r="G5" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="P5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" s="29" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" s="29" t="n">
         <v>1</v>
       </c>
       <c r="W5" s="22" t="n">
@@ -3868,7 +3878,7 @@
     </row>
     <row r="6" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20"/>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="21" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -3889,40 +3899,40 @@
       <c r="H6" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="I6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="J6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="K6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="L6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="M6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="N6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="O6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="P6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="R6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="S6" s="24" t="n">
-        <v>3</v>
-      </c>
-      <c r="T6" s="24" t="n">
+      <c r="I6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="L6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="M6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="N6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="O6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="P6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="R6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="S6" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="T6" s="25" t="n">
         <v>3</v>
       </c>
       <c r="U6" s="24" t="n">
@@ -3937,7 +3947,7 @@
     </row>
     <row r="7" customFormat="false" ht="37.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20"/>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="21" t="s">
         <v>52</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -3958,46 +3968,46 @@
       <c r="H7" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="I7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="J7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="K7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="L7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="M7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="N7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="O7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="P7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="R7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="S7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="T7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="U7" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="V7" s="24" t="n">
+      <c r="I7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="J7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="K7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="L7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="M7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="N7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="O7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="P7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="R7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="S7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="T7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="U7" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="V7" s="25" t="n">
         <v>4</v>
       </c>
       <c r="W7" s="24" t="n">
@@ -4006,7 +4016,7 @@
     </row>
     <row r="8" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20"/>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="21" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -4018,13 +4028,13 @@
       <c r="E8" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="F8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="F8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="22" t="n">
         <v>0</v>
       </c>
       <c r="I8" s="24" t="n">
@@ -4075,7 +4085,7 @@
     </row>
     <row r="9" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20"/>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="21" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -4144,7 +4154,7 @@
     </row>
     <row r="10" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20"/>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -4168,43 +4178,43 @@
       <c r="I10" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="J10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="K10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="L10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="M10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="N10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="O10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="P10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="R10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="S10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="T10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="U10" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="V10" s="24" t="n">
+      <c r="J10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="K10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="L10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="M10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="N10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="O10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="P10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="R10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="S10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="T10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="U10" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="V10" s="25" t="n">
         <v>4</v>
       </c>
       <c r="W10" s="24" t="n">
@@ -4213,7 +4223,7 @@
     </row>
     <row r="11" customFormat="false" ht="37.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="26" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -4240,40 +4250,40 @@
       <c r="J11" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="K11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="L11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="M11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="N11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="O11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="P11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="R11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="S11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="T11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="U11" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="V11" s="24" t="n">
+      <c r="K11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="L11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="M11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="N11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="O11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="P11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="R11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="S11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="T11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="U11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="V11" s="25" t="n">
         <v>1</v>
       </c>
       <c r="W11" s="24" t="n">
@@ -4284,7 +4294,7 @@
       <c r="A12" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="32" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="33" t="s">
@@ -4344,7 +4354,7 @@
       <c r="U12" s="34" t="n">
         <v>3</v>
       </c>
-      <c r="V12" s="36" t="n">
+      <c r="V12" s="35" t="n">
         <v>3</v>
       </c>
       <c r="W12" s="36" t="n">
@@ -4353,7 +4363,7 @@
     </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="37" t="s">
         <v>59</v>
       </c>
       <c r="C13" s="38" t="s">
@@ -4413,7 +4423,7 @@
       <c r="U13" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="V13" s="40" t="n">
+      <c r="V13" s="28" t="n">
         <v>1</v>
       </c>
       <c r="W13" s="40" t="n">
@@ -4422,7 +4432,7 @@
     </row>
     <row r="14" customFormat="false" ht="33.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="20"/>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="37" t="s">
         <v>60</v>
       </c>
       <c r="C14" s="38" t="s">
@@ -4458,31 +4468,31 @@
       <c r="M14" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="N14" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="O14" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="P14" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="R14" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="S14" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="T14" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="U14" s="22" t="n">
-        <v>2</v>
-      </c>
-      <c r="V14" s="22" t="n">
+      <c r="N14" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="O14" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="R14" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="S14" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="T14" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="U14" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="V14" s="29" t="n">
         <v>2</v>
       </c>
       <c r="W14" s="22" t="n">

</xml_diff>

<commit_message>
azurirana tablica i dodan stomp client
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>New estimates of effort remaining as of sprint</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Brisanje grupe</t>
   </si>
   <si>
-    <t>Dodavanje ljudi u grupu prek korisničko imena</t>
-  </si>
-  <si>
     <t>Pregled lokacija ljudi iz grupe</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Dodavanje preko NFC-a</t>
   </si>
   <si>
-    <t>Brojač ljudi</t>
-  </si>
-  <si>
     <t>Sprint 1</t>
   </si>
   <si>
@@ -204,7 +198,7 @@
     <t>izraditi logiku za povijest grupa</t>
   </si>
   <si>
-    <t>Dodavanje u grupu preko korisničkog imena</t>
+    <t>Dodavanje u grupu samostalno (kodom)</t>
   </si>
   <si>
     <t>Napraviti logiku dodavanja u grupu na mobilnom uređaju</t>
@@ -213,9 +207,6 @@
     <t>Napraviti module za dodavanje u grupu</t>
   </si>
   <si>
-    <t>Dodavanje u grupu samostalno (kodom)</t>
-  </si>
-  <si>
     <t>Napraviti logiku web servisa za dodavanje ljudi u grupu</t>
   </si>
   <si>
@@ -234,7 +225,10 @@
     <t>Dodavanje u grupu NFC-om</t>
   </si>
   <si>
-    <t>Napraviti NFC beam aktivnost za razmjenu koda</t>
+    <t>NFC beam aktivnost (UI)</t>
+  </si>
+  <si>
+    <t>NFC beam aktivnost (logika)</t>
   </si>
 </sst>
 </file>
@@ -246,7 +240,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -331,11 +325,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -369,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -482,6 +471,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="medium"/>
+      <right/>
+      <top/>
+      <bottom style="medium"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -508,7 +504,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -681,24 +677,32 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -773,7 +777,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1151,11 +1155,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="96322972"/>
-        <c:axId val="17505846"/>
+        <c:axId val="82941613"/>
+        <c:axId val="7906172"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="96322972"/>
+        <c:axId val="82941613"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1195,14 +1199,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="17505846"/>
+        <c:crossAx val="7906172"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17505846"/>
+        <c:axId val="7906172"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1252,7 +1256,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96322972"/>
+        <c:crossAx val="82941613"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1287,7 +1291,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1662,11 +1666,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="45119683"/>
-        <c:axId val="6675984"/>
+        <c:axId val="47888192"/>
+        <c:axId val="68856703"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45119683"/>
+        <c:axId val="47888192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1682,14 +1686,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="6675984"/>
+        <c:crossAx val="68856703"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6675984"/>
+        <c:axId val="68856703"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1718,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45119683"/>
+        <c:crossAx val="47888192"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1749,7 +1753,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1763,7 +1767,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300">
+              <a:rPr b="1" sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Burndown chart</a:t>
@@ -1803,7 +1807,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1976,7 +1980,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="7"/>
+            <c:size val="6"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -2124,11 +2128,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="10499988"/>
-        <c:axId val="17085414"/>
+        <c:axId val="95479977"/>
+        <c:axId val="89703723"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="10499988"/>
+        <c:axId val="95479977"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2144,14 +2148,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="17085414"/>
-        <c:crossesAt val="0"/>
+        <c:crossAx val="89703723"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="17085414"/>
+        <c:axId val="89703723"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2176,7 +2180,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="10499988"/>
+        <c:crossAx val="95479977"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2216,15 +2220,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2180160</xdr:colOff>
+      <xdr:colOff>2207160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>106200</xdr:rowOff>
+      <xdr:rowOff>97200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1170360</xdr:colOff>
+      <xdr:colOff>1197000</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>14400</xdr:rowOff>
+      <xdr:rowOff>5040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2232,8 +2236,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2180160" y="7156440"/>
-        <a:ext cx="9964800" cy="5623200"/>
+        <a:off x="2207160" y="7147440"/>
+        <a:ext cx="9964440" cy="5622840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2251,15 +2255,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>33120</xdr:colOff>
+      <xdr:colOff>60120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>308520</xdr:rowOff>
+      <xdr:rowOff>299520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>635040</xdr:colOff>
+      <xdr:colOff>661680</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>53280</xdr:rowOff>
+      <xdr:rowOff>43920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2267,8 +2271,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2542320" y="7084440"/>
-        <a:ext cx="9043920" cy="4305960"/>
+        <a:off x="2569320" y="7075440"/>
+        <a:ext cx="9043560" cy="4305600"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2286,15 +2290,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:colOff>63360</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>27000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>646200</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>24480</xdr:rowOff>
+      <xdr:colOff>672840</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2302,8 +2306,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4002480" y="4579920"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="4029480" y="5066280"/>
+        <a:ext cx="5759280" cy="3239640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2321,15 +2325,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="36.2834008097166"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.4858299595142"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.7125506072874"/>
@@ -2468,7 +2472,7 @@
       <c r="H6" s="7"/>
       <c r="I6" s="6"/>
     </row>
-    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -2476,16 +2480,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="E7" s="7" t="n">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F7" s="7" t="n">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -2499,16 +2503,16 @@
         <v>6</v>
       </c>
       <c r="C8" s="6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="E8" s="7" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="F8" s="7" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
@@ -2522,22 +2526,22 @@
         <v>7</v>
       </c>
       <c r="C9" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D9" s="6" t="n">
         <v>6</v>
       </c>
-      <c r="D9" s="6" t="n">
-        <v>22</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>22</v>
-      </c>
-      <c r="F9" s="7" t="n">
-        <v>22</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
+      <c r="E9" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
       <c r="I9" s="6"/>
     </row>
-    <row r="10" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -2545,22 +2549,22 @@
         <v>8</v>
       </c>
       <c r="C10" s="6" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>6</v>
-      </c>
-      <c r="E10" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="F10" s="8" t="n">
-        <v>6</v>
-      </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
+        <v>8</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="6"/>
     </row>
-    <row r="11" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
@@ -2568,67 +2572,23 @@
         <v>9</v>
       </c>
       <c r="C11" s="6" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D11" s="6" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E11" s="7" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F11" s="7" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="6"/>
     </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="6" t="n">
-        <v>10</v>
-      </c>
-      <c r="C12" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="D12" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="E12" s="7" t="n">
-        <v>16</v>
-      </c>
-      <c r="F12" s="7" t="n">
-        <v>16</v>
-      </c>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="6" t="n">
-        <v>11</v>
-      </c>
-      <c r="C13" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D13" s="6" t="n">
-        <v>4</v>
-      </c>
-      <c r="E13" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="F13" s="7" t="n">
-        <v>4</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="6"/>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="E1:H1"/>
@@ -2648,10 +2608,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2663,7 +2623,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>5</v>
@@ -2677,7 +2637,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>7</v>
@@ -2689,58 +2649,48 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="13"/>
+      <c r="B6" s="11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="13"/>
-      <c r="B7" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="10" t="s">
+    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13"/>
+      <c r="B8" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="13"/>
       <c r="B9" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="13"/>
-      <c r="B11" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A7:A9"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -2779,7 +2729,7 @@
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="E1" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
@@ -2802,13 +2752,13 @@
     </row>
     <row r="2" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>4</v>
@@ -2876,10 +2826,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>1</v>
@@ -2945,10 +2895,10 @@
     <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20"/>
       <c r="B4" s="21" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>1</v>
@@ -3014,10 +2964,10 @@
     <row r="5" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20"/>
       <c r="B5" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>1</v>
@@ -3083,10 +3033,10 @@
     <row r="6" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="20"/>
       <c r="B6" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>1</v>
@@ -3152,10 +3102,10 @@
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="20"/>
       <c r="B7" s="21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>1</v>
@@ -3221,10 +3171,10 @@
     <row r="8" customFormat="false" ht="31.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20"/>
       <c r="B8" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>2</v>
@@ -3290,10 +3240,10 @@
     <row r="9" customFormat="false" ht="30.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20"/>
       <c r="B9" s="26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="6" t="n">
         <v>2</v>
@@ -3360,10 +3310,10 @@
     <row r="10" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20"/>
       <c r="B10" s="27" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D10" s="6" t="n">
         <v>4</v>
@@ -3429,10 +3379,10 @@
     <row r="11" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
       <c r="B11" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6" t="n">
         <v>2</v>
@@ -3498,10 +3448,10 @@
     <row r="12" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="20"/>
       <c r="B12" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D12" s="6" t="n">
         <v>2</v>
@@ -3567,10 +3517,10 @@
     <row r="13" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
       <c r="B13" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="6" t="n">
         <v>2</v>
@@ -3636,10 +3586,10 @@
     <row r="14" customFormat="false" ht="31.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="20"/>
       <c r="B14" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D14" s="6" t="n">
         <v>4</v>
@@ -3707,10 +3657,10 @@
         <v>6</v>
       </c>
       <c r="B15" s="32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D15" s="33" t="n">
         <v>3</v>
@@ -3776,10 +3726,10 @@
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20"/>
       <c r="B16" s="37" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="38" t="n">
         <v>3</v>
@@ -3845,10 +3795,10 @@
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20"/>
       <c r="B17" s="37" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D17" s="38" t="n">
         <v>1</v>
@@ -3913,7 +3863,7 @@
     </row>
     <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="41"/>
       <c r="C18" s="41"/>
@@ -4000,7 +3950,7 @@
     </row>
     <row r="19" customFormat="false" ht="30.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="41"/>
       <c r="C19" s="41"/>
@@ -4111,7 +4061,7 @@
   </sheetPr>
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="P11" activeCellId="0" sqref="P11"/>
     </sheetView>
   </sheetViews>
@@ -4131,7 +4081,7 @@
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="E1" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F1" s="17"/>
       <c r="G1" s="17"/>
@@ -4154,13 +4104,13 @@
     </row>
     <row r="2" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>21</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>4</v>
@@ -4228,10 +4178,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" s="6" t="n">
         <v>3</v>
@@ -4297,10 +4247,10 @@
     <row r="4" customFormat="false" ht="27.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20"/>
       <c r="B4" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>2</v>
@@ -4366,10 +4316,10 @@
     <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="20"/>
       <c r="B5" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>1</v>
@@ -4435,10 +4385,10 @@
     <row r="6" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20"/>
       <c r="B6" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>3</v>
@@ -4504,10 +4454,10 @@
     <row r="7" customFormat="false" ht="37.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20"/>
       <c r="B7" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>4</v>
@@ -4573,10 +4523,10 @@
     <row r="8" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20"/>
       <c r="B8" s="21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>1</v>
@@ -4642,10 +4592,10 @@
     <row r="9" customFormat="false" ht="31.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20"/>
       <c r="B9" s="21" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D9" s="6" t="n">
         <v>1</v>
@@ -4711,10 +4661,10 @@
     <row r="10" customFormat="false" ht="39.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20"/>
       <c r="B10" s="21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="6" t="n">
         <v>4</v>
@@ -4780,10 +4730,10 @@
     <row r="11" customFormat="false" ht="37.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
       <c r="B11" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6" t="n">
         <v>2</v>
@@ -4851,10 +4801,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D12" s="33" t="n">
         <v>3</v>
@@ -4920,10 +4870,10 @@
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
       <c r="B13" s="37" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C13" s="38" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D13" s="38" t="n">
         <v>1</v>
@@ -4989,10 +4939,10 @@
     <row r="14" customFormat="false" ht="33.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="20"/>
       <c r="B14" s="37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14" s="38" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D14" s="38" t="n">
         <v>2</v>
@@ -5057,7 +5007,7 @@
     </row>
     <row r="15" customFormat="false" ht="36.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="41"/>
       <c r="C15" s="41"/>
@@ -5144,7 +5094,7 @@
     </row>
     <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="41" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" s="41"/>
       <c r="C16" s="41"/>
@@ -5254,10 +5204,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN11"/>
+  <dimension ref="A1:AN12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5282,13 +5232,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>21</v>
-      </c>
-      <c r="B1" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>23</v>
       </c>
       <c r="D1" s="18" t="s">
         <v>4</v>
@@ -5353,20 +5303,26 @@
     </row>
     <row r="2" customFormat="false" ht="33.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" s="6" t="n">
         <v>6</v>
       </c>
       <c r="E2" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
+      <c r="F2" s="23" t="n">
+        <v>6</v>
+      </c>
+      <c r="G2" s="23" t="n">
+        <v>6</v>
+      </c>
       <c r="H2" s="29"/>
       <c r="I2" s="29"/>
       <c r="J2" s="29"/>
@@ -5387,17 +5343,23 @@
     <row r="3" customFormat="false" ht="33.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20"/>
       <c r="B3" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="6"/>
+        <v>61</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="D3" s="6" t="n">
         <v>3</v>
       </c>
       <c r="E3" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>3</v>
+      </c>
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
       <c r="K3" s="25"/>
@@ -5415,45 +5377,49 @@
       <c r="W3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43" t="n">
+      <c r="A4" s="20"/>
+      <c r="B4" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="E4" s="33" t="n">
+      <c r="E4" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
+      <c r="F4" s="38" t="n">
+        <v>5</v>
+      </c>
+      <c r="G4" s="38" t="n">
+        <v>5</v>
+      </c>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="25.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20"/>
       <c r="B5" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>4</v>
@@ -5520,17 +5486,23 @@
     <row r="6" customFormat="false" ht="33.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="20"/>
       <c r="B6" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" s="6"/>
+        <v>64</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>23</v>
+      </c>
       <c r="D6" s="6" t="n">
         <v>3</v>
       </c>
       <c r="E6" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
+      <c r="F6" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" s="23" t="n">
+        <v>3</v>
+      </c>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
       <c r="J6" s="21"/>
@@ -5551,10 +5523,10 @@
     <row r="7" customFormat="false" ht="25.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20"/>
       <c r="B7" s="23" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>2</v>
@@ -5620,11 +5592,11 @@
     </row>
     <row r="8" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20"/>
-      <c r="B8" s="46" t="s">
-        <v>69</v>
+      <c r="B8" s="43" t="s">
+        <v>66</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>4</v>
@@ -5632,8 +5604,12 @@
       <c r="E8" s="23" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
+      <c r="F8" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>4</v>
+      </c>
       <c r="I8" s="25"/>
       <c r="J8" s="25"/>
       <c r="K8" s="25"/>
@@ -5652,20 +5628,26 @@
     </row>
     <row r="9" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B9" s="47" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="33"/>
+        <v>67</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>27</v>
+      </c>
       <c r="D9" s="33" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E9" s="33" t="n">
-        <v>8</v>
-      </c>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
+        <v>4</v>
+      </c>
+      <c r="F9" s="33" t="n">
+        <v>4</v>
+      </c>
+      <c r="G9" s="33" t="n">
+        <v>4</v>
+      </c>
       <c r="H9" s="34"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
@@ -5683,186 +5665,223 @@
       <c r="V9" s="35"/>
       <c r="W9" s="36"/>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="41"/>
-      <c r="C10" s="41"/>
-      <c r="D10" s="0" t="n">
-        <f aca="false">SUM(D2:D9)</f>
-        <v>35</v>
-      </c>
-      <c r="E10" s="42" t="n">
-        <f aca="false">D10-($D$10/19)</f>
-        <v>33.1578947368421</v>
-      </c>
-      <c r="F10" s="42" t="n">
-        <f aca="false">E10-($D$10/19)</f>
-        <v>31.3157894736842</v>
-      </c>
-      <c r="G10" s="42" t="n">
-        <f aca="false">F10-($D$10/19)</f>
-        <v>29.4736842105263</v>
-      </c>
-      <c r="H10" s="42" t="n">
-        <f aca="false">G10-($D$10/19)</f>
-        <v>27.6315789473684</v>
-      </c>
-      <c r="I10" s="42" t="n">
-        <f aca="false">H10-($D$10/19)</f>
-        <v>25.7894736842105</v>
-      </c>
-      <c r="J10" s="42" t="n">
-        <f aca="false">I10-($D$10/19)</f>
-        <v>23.9473684210526</v>
-      </c>
-      <c r="K10" s="42" t="n">
-        <f aca="false">J10-($D$10/19)</f>
-        <v>22.1052631578947</v>
-      </c>
-      <c r="L10" s="42" t="n">
-        <f aca="false">K10-($D$10/19)</f>
-        <v>20.2631578947368</v>
-      </c>
-      <c r="M10" s="42" t="n">
-        <f aca="false">L10-($D$10/19)</f>
-        <v>18.421052631579</v>
-      </c>
-      <c r="N10" s="42" t="n">
-        <f aca="false">M10-($D$10/19)</f>
-        <v>16.5789473684211</v>
-      </c>
-      <c r="O10" s="42" t="n">
-        <f aca="false">N10-($D$10/19)</f>
-        <v>14.7368421052632</v>
-      </c>
-      <c r="P10" s="42" t="n">
-        <f aca="false">O10-($D$10/19)</f>
-        <v>12.8947368421053</v>
-      </c>
-      <c r="Q10" s="42" t="n">
-        <f aca="false">P10-($D$10/19)</f>
-        <v>11.0526315789474</v>
-      </c>
-      <c r="R10" s="42" t="n">
-        <f aca="false">Q10-($D$10/19)</f>
-        <v>9.21052631578948</v>
-      </c>
-      <c r="S10" s="42" t="n">
-        <f aca="false">R10-($D$10/19)</f>
-        <v>7.36842105263159</v>
-      </c>
-      <c r="T10" s="42" t="n">
-        <f aca="false">S10-($D$10/19)</f>
-        <v>5.52631578947369</v>
-      </c>
-      <c r="U10" s="42" t="n">
-        <f aca="false">T10-($D$10/19)</f>
-        <v>3.6842105263158</v>
-      </c>
-      <c r="V10" s="42" t="n">
-        <f aca="false">U10-($D$10/19)</f>
-        <v>1.8421052631579</v>
-      </c>
-      <c r="W10" s="42" t="n">
-        <f aca="false">V10-($D$10/19)</f>
-        <v>9.76996261670138E-015</v>
-      </c>
+    <row r="10" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20"/>
+      <c r="B10" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="46" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" s="46" t="n">
+        <v>4</v>
+      </c>
+      <c r="F10" s="46" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" s="46" t="n">
+        <v>4</v>
+      </c>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="47"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+      <c r="P10" s="47"/>
+      <c r="Q10" s="47"/>
+      <c r="R10" s="47"/>
+      <c r="S10" s="47"/>
+      <c r="T10" s="47"/>
+      <c r="U10" s="47"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="49"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="41" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B11" s="41"/>
       <c r="C11" s="41"/>
       <c r="D11" s="0" t="n">
         <f aca="false">SUM(D2:D9)</f>
-        <v>35</v>
-      </c>
-      <c r="E11" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="E11" s="42" t="n">
+        <f aca="false">D11-($D$11/19)</f>
+        <v>29.3684210526316</v>
+      </c>
+      <c r="F11" s="42" t="n">
+        <f aca="false">E11-($D$11/19)</f>
+        <v>27.7368421052632</v>
+      </c>
+      <c r="G11" s="42" t="n">
+        <f aca="false">F11-($D$11/19)</f>
+        <v>26.1052631578947</v>
+      </c>
+      <c r="H11" s="42" t="n">
+        <f aca="false">G11-($D$11/19)</f>
+        <v>24.4736842105263</v>
+      </c>
+      <c r="I11" s="42" t="n">
+        <f aca="false">H11-($D$11/19)</f>
+        <v>22.8421052631579</v>
+      </c>
+      <c r="J11" s="42" t="n">
+        <f aca="false">I11-($D$11/19)</f>
+        <v>21.2105263157895</v>
+      </c>
+      <c r="K11" s="42" t="n">
+        <f aca="false">J11-($D$11/19)</f>
+        <v>19.5789473684211</v>
+      </c>
+      <c r="L11" s="42" t="n">
+        <f aca="false">K11-($D$11/19)</f>
+        <v>17.9473684210526</v>
+      </c>
+      <c r="M11" s="42" t="n">
+        <f aca="false">L11-($D$11/19)</f>
+        <v>16.3157894736842</v>
+      </c>
+      <c r="N11" s="42" t="n">
+        <f aca="false">M11-($D$11/19)</f>
+        <v>14.6842105263158</v>
+      </c>
+      <c r="O11" s="42" t="n">
+        <f aca="false">N11-($D$11/19)</f>
+        <v>13.0526315789474</v>
+      </c>
+      <c r="P11" s="42" t="n">
+        <f aca="false">O11-($D$11/19)</f>
+        <v>11.4210526315789</v>
+      </c>
+      <c r="Q11" s="42" t="n">
+        <f aca="false">P11-($D$11/19)</f>
+        <v>9.78947368421052</v>
+      </c>
+      <c r="R11" s="42" t="n">
+        <f aca="false">Q11-($D$11/19)</f>
+        <v>8.1578947368421</v>
+      </c>
+      <c r="S11" s="42" t="n">
+        <f aca="false">R11-($D$11/19)</f>
+        <v>6.52631578947368</v>
+      </c>
+      <c r="T11" s="42" t="n">
+        <f aca="false">S11-($D$11/19)</f>
+        <v>4.89473684210526</v>
+      </c>
+      <c r="U11" s="42" t="n">
+        <f aca="false">T11-($D$11/19)</f>
+        <v>3.26315789473684</v>
+      </c>
+      <c r="V11" s="42" t="n">
+        <f aca="false">U11-($D$11/19)</f>
+        <v>1.63157894736842</v>
+      </c>
+      <c r="W11" s="42" t="n">
+        <f aca="false">V11-($D$11/19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="41"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="0" t="n">
+        <f aca="false">SUM(D2:D9)</f>
+        <v>31</v>
+      </c>
+      <c r="E12" s="0" t="n">
         <f aca="false">SUM(E2:E9)</f>
-        <v>29</v>
-      </c>
-      <c r="F11" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="F12" s="0" t="n">
         <f aca="false">SUM(F2:F9)</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <f aca="false">SUM(G2:G9)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="H12" s="0" t="n">
         <f aca="false">SUM(H2:H9)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="0" t="n">
+      <c r="I12" s="0" t="n">
         <f aca="false">SUM(I2:I9)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="0" t="n">
+      <c r="J12" s="0" t="n">
         <f aca="false">SUM(J2:J9)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="0" t="n">
+      <c r="K12" s="0" t="n">
         <f aca="false">SUM(K2:K9)</f>
         <v>0</v>
       </c>
-      <c r="L11" s="0" t="n">
+      <c r="L12" s="0" t="n">
         <f aca="false">SUM(L2:L9)</f>
         <v>0</v>
       </c>
-      <c r="M11" s="0" t="n">
+      <c r="M12" s="0" t="n">
         <f aca="false">SUM(M2:M9)</f>
         <v>0</v>
       </c>
-      <c r="N11" s="0" t="n">
+      <c r="N12" s="0" t="n">
         <f aca="false">SUM(N2:N9)</f>
         <v>0</v>
       </c>
-      <c r="O11" s="0" t="n">
+      <c r="O12" s="0" t="n">
         <f aca="false">SUM(O2:O9)</f>
         <v>0</v>
       </c>
-      <c r="P11" s="0" t="n">
+      <c r="P12" s="0" t="n">
         <f aca="false">SUM(P2:P9)</f>
         <v>0</v>
       </c>
-      <c r="Q11" s="0" t="n">
+      <c r="Q12" s="0" t="n">
         <f aca="false">SUM(Q2:Q9)</f>
         <v>0</v>
       </c>
-      <c r="R11" s="0" t="n">
+      <c r="R12" s="0" t="n">
         <f aca="false">SUM(R2:R9)</f>
         <v>0</v>
       </c>
-      <c r="S11" s="0" t="n">
+      <c r="S12" s="0" t="n">
         <f aca="false">SUM(S2:S9)</f>
         <v>0</v>
       </c>
-      <c r="T11" s="0" t="n">
+      <c r="T12" s="0" t="n">
         <f aca="false">SUM(T2:T9)</f>
         <v>0</v>
       </c>
-      <c r="U11" s="0" t="n">
+      <c r="U12" s="0" t="n">
         <f aca="false">SUM(U2:U9)</f>
         <v>0</v>
       </c>
-      <c r="V11" s="0" t="n">
+      <c r="V12" s="0" t="n">
         <f aca="false">SUM(V2:V9)</f>
         <v>0</v>
       </c>
-      <c r="W11" s="0" t="n">
+      <c r="W12" s="0" t="n">
         <f aca="false">SUM(W2:W9)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A12:C12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
created nfc animations, first team fragment and required layouts, fixed some warnings and replaced values with dimens in layouts
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
   <si>
     <t>New estimates of effort remaining as of sprint</t>
   </si>
@@ -226,6 +226,9 @@
   </si>
   <si>
     <t>NFC beam aktivnost (UI)</t>
+  </si>
+  <si>
+    <t>Napraviti animaciju za NFC beam</t>
   </si>
   <si>
     <t>NFC beam aktivnost (logika)</t>
@@ -504,7 +507,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -685,6 +688,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -777,7 +784,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1155,11 +1162,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="82941613"/>
-        <c:axId val="7906172"/>
+        <c:axId val="11239909"/>
+        <c:axId val="56335224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82941613"/>
+        <c:axId val="11239909"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1199,14 +1206,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="7906172"/>
+        <c:crossAx val="56335224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7906172"/>
+        <c:axId val="56335224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1256,7 +1263,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82941613"/>
+        <c:crossAx val="11239909"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1291,7 +1298,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1666,11 +1673,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="47888192"/>
-        <c:axId val="68856703"/>
+        <c:axId val="73296840"/>
+        <c:axId val="45880741"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47888192"/>
+        <c:axId val="73296840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1686,14 +1693,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68856703"/>
+        <c:crossAx val="45880741"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="68856703"/>
+        <c:axId val="45880741"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1718,7 +1725,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="47888192"/>
+        <c:crossAx val="73296840"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1753,7 +1760,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1807,7 +1814,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1980,7 +1987,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="6"/>
+            <c:size val="5"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -2128,11 +2135,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95479977"/>
-        <c:axId val="89703723"/>
+        <c:axId val="5998308"/>
+        <c:axId val="72652294"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95479977"/>
+        <c:axId val="5998308"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2148,14 +2155,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="89703723"/>
+        <c:crossAx val="72652294"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89703723"/>
+        <c:axId val="72652294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2180,7 +2187,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="95479977"/>
+        <c:crossAx val="5998308"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2220,15 +2227,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2207160</xdr:colOff>
+      <xdr:colOff>2234160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>88200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1197000</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>5040</xdr:rowOff>
+      <xdr:colOff>1223640</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>186120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2236,8 +2243,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2207160" y="7147440"/>
-        <a:ext cx="9964440" cy="5622840"/>
+        <a:off x="2234160" y="7138440"/>
+        <a:ext cx="9964080" cy="5622480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2255,15 +2262,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>60120</xdr:colOff>
+      <xdr:colOff>87120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>299520</xdr:rowOff>
+      <xdr:rowOff>290520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>661680</xdr:colOff>
+      <xdr:colOff>688320</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>43920</xdr:rowOff>
+      <xdr:rowOff>34560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2271,8 +2278,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2569320" y="7075440"/>
-        <a:ext cx="9043560" cy="4305600"/>
+        <a:off x="2596320" y="7066440"/>
+        <a:ext cx="9043200" cy="4305240"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2290,15 +2297,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>63360</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>27000</xdr:rowOff>
+      <xdr:colOff>90360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>18000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>672840</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>15480</xdr:rowOff>
+      <xdr:colOff>699480</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2306,8 +2313,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4029480" y="5066280"/>
-        <a:ext cx="5759280" cy="3239640"/>
+        <a:off x="4056480" y="5552640"/>
+        <a:ext cx="5758920" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5204,10 +5211,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN12"/>
+  <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5323,9 +5330,15 @@
       <c r="G2" s="23" t="n">
         <v>6</v>
       </c>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
+      <c r="H2" s="29" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2" s="29" t="n">
+        <v>6</v>
+      </c>
+      <c r="J2" s="29" t="n">
+        <v>6</v>
+      </c>
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
@@ -5360,8 +5373,15 @@
       <c r="G3" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
+      <c r="H3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" s="25" t="n">
+        <v>3</v>
+      </c>
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
       <c r="M3" s="25"/>
@@ -5396,9 +5416,15 @@
       <c r="G4" s="38" t="n">
         <v>5</v>
       </c>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
+      <c r="H4" s="25" t="n">
+        <v>5</v>
+      </c>
+      <c r="I4" s="25" t="n">
+        <v>5</v>
+      </c>
+      <c r="J4" s="25" t="n">
+        <v>5</v>
+      </c>
       <c r="K4" s="24"/>
       <c r="L4" s="24"/>
       <c r="M4" s="24"/>
@@ -5503,9 +5529,15 @@
       <c r="G6" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="H6" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" s="23" t="n">
+        <v>3</v>
+      </c>
+      <c r="J6" s="23" t="n">
+        <v>3</v>
+      </c>
       <c r="K6" s="21"/>
       <c r="L6" s="21"/>
       <c r="M6" s="21"/>
@@ -5610,21 +5642,54 @@
       <c r="G8" s="6" t="n">
         <v>4</v>
       </c>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="O8" s="25"/>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-      <c r="W8" s="24"/>
+      <c r="H8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I8" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="J8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W8" s="24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20" t="s">
@@ -5637,20 +5702,26 @@
         <v>27</v>
       </c>
       <c r="D9" s="33" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="33" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" s="33" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G9" s="33" t="n">
-        <v>4</v>
-      </c>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+        <v>2</v>
+      </c>
+      <c r="H9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="34" t="n">
+        <v>2</v>
+      </c>
       <c r="K9" s="35"/>
       <c r="L9" s="34"/>
       <c r="M9" s="34"/>
@@ -5670,208 +5741,283 @@
       <c r="B10" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V10" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W10" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="20"/>
+      <c r="B11" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="46" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" s="46" t="n">
-        <v>4</v>
-      </c>
-      <c r="F10" s="46" t="n">
-        <v>4</v>
-      </c>
-      <c r="G10" s="46" t="n">
-        <v>4</v>
-      </c>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
-      <c r="J10" s="47"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="47"/>
-      <c r="M10" s="47"/>
-      <c r="N10" s="47"/>
-      <c r="O10" s="47"/>
-      <c r="P10" s="47"/>
-      <c r="Q10" s="47"/>
-      <c r="R10" s="47"/>
-      <c r="S10" s="47"/>
-      <c r="T10" s="47"/>
-      <c r="U10" s="47"/>
-      <c r="V10" s="48"/>
-      <c r="W10" s="49"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="41"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="0" t="n">
-        <f aca="false">SUM(D2:D9)</f>
-        <v>31</v>
-      </c>
-      <c r="E11" s="42" t="n">
-        <f aca="false">D11-($D$11/19)</f>
-        <v>29.3684210526316</v>
-      </c>
-      <c r="F11" s="42" t="n">
-        <f aca="false">E11-($D$11/19)</f>
-        <v>27.7368421052632</v>
-      </c>
-      <c r="G11" s="42" t="n">
-        <f aca="false">F11-($D$11/19)</f>
-        <v>26.1052631578947</v>
-      </c>
-      <c r="H11" s="42" t="n">
-        <f aca="false">G11-($D$11/19)</f>
-        <v>24.4736842105263</v>
-      </c>
-      <c r="I11" s="42" t="n">
-        <f aca="false">H11-($D$11/19)</f>
-        <v>22.8421052631579</v>
-      </c>
-      <c r="J11" s="42" t="n">
-        <f aca="false">I11-($D$11/19)</f>
-        <v>21.2105263157895</v>
-      </c>
-      <c r="K11" s="42" t="n">
-        <f aca="false">J11-($D$11/19)</f>
-        <v>19.5789473684211</v>
-      </c>
-      <c r="L11" s="42" t="n">
-        <f aca="false">K11-($D$11/19)</f>
-        <v>17.9473684210526</v>
-      </c>
-      <c r="M11" s="42" t="n">
-        <f aca="false">L11-($D$11/19)</f>
-        <v>16.3157894736842</v>
-      </c>
-      <c r="N11" s="42" t="n">
-        <f aca="false">M11-($D$11/19)</f>
-        <v>14.6842105263158</v>
-      </c>
-      <c r="O11" s="42" t="n">
-        <f aca="false">N11-($D$11/19)</f>
-        <v>13.0526315789474</v>
-      </c>
-      <c r="P11" s="42" t="n">
-        <f aca="false">O11-($D$11/19)</f>
-        <v>11.4210526315789</v>
-      </c>
-      <c r="Q11" s="42" t="n">
-        <f aca="false">P11-($D$11/19)</f>
-        <v>9.78947368421052</v>
-      </c>
-      <c r="R11" s="42" t="n">
-        <f aca="false">Q11-($D$11/19)</f>
-        <v>8.1578947368421</v>
-      </c>
-      <c r="S11" s="42" t="n">
-        <f aca="false">R11-($D$11/19)</f>
-        <v>6.52631578947368</v>
-      </c>
-      <c r="T11" s="42" t="n">
-        <f aca="false">S11-($D$11/19)</f>
-        <v>4.89473684210526</v>
-      </c>
-      <c r="U11" s="42" t="n">
-        <f aca="false">T11-($D$11/19)</f>
-        <v>3.26315789473684</v>
-      </c>
-      <c r="V11" s="42" t="n">
-        <f aca="false">U11-($D$11/19)</f>
-        <v>1.63157894736842</v>
-      </c>
-      <c r="W11" s="42" t="n">
-        <f aca="false">V11-($D$11/19)</f>
-        <v>0</v>
-      </c>
+      <c r="D11" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="E11" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="F11" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" s="48" t="n">
+        <v>4</v>
+      </c>
+      <c r="I11" s="48" t="n">
+        <v>4</v>
+      </c>
+      <c r="J11" s="48" t="n">
+        <v>4</v>
+      </c>
+      <c r="K11" s="49"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="49"/>
+      <c r="W11" s="50"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="41"/>
       <c r="C12" s="41"/>
       <c r="D12" s="0" t="n">
         <f aca="false">SUM(D2:D9)</f>
-        <v>31</v>
-      </c>
-      <c r="E12" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="E12" s="42" t="n">
+        <f aca="false">D12-($D$12/19)</f>
+        <v>27.4736842105263</v>
+      </c>
+      <c r="F12" s="42" t="n">
+        <f aca="false">E12-($D$12/19)</f>
+        <v>25.9473684210526</v>
+      </c>
+      <c r="G12" s="42" t="n">
+        <f aca="false">F12-($D$12/19)</f>
+        <v>24.4210526315789</v>
+      </c>
+      <c r="H12" s="42" t="n">
+        <f aca="false">G12-($D$12/19)</f>
+        <v>22.8947368421053</v>
+      </c>
+      <c r="I12" s="42" t="n">
+        <f aca="false">H12-($D$12/19)</f>
+        <v>21.3684210526316</v>
+      </c>
+      <c r="J12" s="42" t="n">
+        <f aca="false">I12-($D$12/19)</f>
+        <v>19.8421052631579</v>
+      </c>
+      <c r="K12" s="42" t="n">
+        <f aca="false">J12-($D$12/19)</f>
+        <v>18.3157894736842</v>
+      </c>
+      <c r="L12" s="42" t="n">
+        <f aca="false">K12-($D$12/19)</f>
+        <v>16.7894736842105</v>
+      </c>
+      <c r="M12" s="42" t="n">
+        <f aca="false">L12-($D$12/19)</f>
+        <v>15.2631578947368</v>
+      </c>
+      <c r="N12" s="42" t="n">
+        <f aca="false">M12-($D$12/19)</f>
+        <v>13.7368421052632</v>
+      </c>
+      <c r="O12" s="42" t="n">
+        <f aca="false">N12-($D$12/19)</f>
+        <v>12.2105263157895</v>
+      </c>
+      <c r="P12" s="42" t="n">
+        <f aca="false">O12-($D$12/19)</f>
+        <v>10.6842105263158</v>
+      </c>
+      <c r="Q12" s="42" t="n">
+        <f aca="false">P12-($D$12/19)</f>
+        <v>9.1578947368421</v>
+      </c>
+      <c r="R12" s="42" t="n">
+        <f aca="false">Q12-($D$12/19)</f>
+        <v>7.63157894736841</v>
+      </c>
+      <c r="S12" s="42" t="n">
+        <f aca="false">R12-($D$12/19)</f>
+        <v>6.10526315789473</v>
+      </c>
+      <c r="T12" s="42" t="n">
+        <f aca="false">S12-($D$12/19)</f>
+        <v>4.57894736842104</v>
+      </c>
+      <c r="U12" s="42" t="n">
+        <f aca="false">T12-($D$12/19)</f>
+        <v>3.05263157894736</v>
+      </c>
+      <c r="V12" s="42" t="n">
+        <f aca="false">U12-($D$12/19)</f>
+        <v>1.52631578947368</v>
+      </c>
+      <c r="W12" s="42" t="n">
+        <f aca="false">V12-($D$12/19)</f>
+        <v>-9.32587340685132E-015</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="0" t="n">
+        <f aca="false">SUM(D2:D9)</f>
+        <v>29</v>
+      </c>
+      <c r="E13" s="0" t="n">
         <f aca="false">SUM(E2:E9)</f>
-        <v>25</v>
-      </c>
-      <c r="F12" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="F13" s="0" t="n">
         <f aca="false">SUM(F2:F9)</f>
-        <v>25</v>
-      </c>
-      <c r="G12" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <f aca="false">SUM(G2:G9)</f>
-        <v>25</v>
-      </c>
-      <c r="H12" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="H13" s="0" t="n">
         <f aca="false">SUM(H2:H9)</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="I13" s="0" t="n">
         <f aca="false">SUM(I2:I9)</f>
-        <v>0</v>
-      </c>
-      <c r="J12" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="J13" s="0" t="n">
         <f aca="false">SUM(J2:J9)</f>
-        <v>0</v>
-      </c>
-      <c r="K12" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="K13" s="0" t="n">
         <f aca="false">SUM(K2:K9)</f>
         <v>0</v>
       </c>
-      <c r="L12" s="0" t="n">
+      <c r="L13" s="0" t="n">
         <f aca="false">SUM(L2:L9)</f>
         <v>0</v>
       </c>
-      <c r="M12" s="0" t="n">
+      <c r="M13" s="0" t="n">
         <f aca="false">SUM(M2:M9)</f>
         <v>0</v>
       </c>
-      <c r="N12" s="0" t="n">
+      <c r="N13" s="0" t="n">
         <f aca="false">SUM(N2:N9)</f>
         <v>0</v>
       </c>
-      <c r="O12" s="0" t="n">
+      <c r="O13" s="0" t="n">
         <f aca="false">SUM(O2:O9)</f>
         <v>0</v>
       </c>
-      <c r="P12" s="0" t="n">
+      <c r="P13" s="0" t="n">
         <f aca="false">SUM(P2:P9)</f>
         <v>0</v>
       </c>
-      <c r="Q12" s="0" t="n">
+      <c r="Q13" s="0" t="n">
         <f aca="false">SUM(Q2:Q9)</f>
         <v>0</v>
       </c>
-      <c r="R12" s="0" t="n">
+      <c r="R13" s="0" t="n">
         <f aca="false">SUM(R2:R9)</f>
         <v>0</v>
       </c>
-      <c r="S12" s="0" t="n">
+      <c r="S13" s="0" t="n">
         <f aca="false">SUM(S2:S9)</f>
         <v>0</v>
       </c>
-      <c r="T12" s="0" t="n">
+      <c r="T13" s="0" t="n">
         <f aca="false">SUM(T2:T9)</f>
         <v>0</v>
       </c>
-      <c r="U12" s="0" t="n">
+      <c r="U13" s="0" t="n">
         <f aca="false">SUM(U2:U9)</f>
         <v>0</v>
       </c>
-      <c r="V12" s="0" t="n">
+      <c r="V13" s="0" t="n">
         <f aca="false">SUM(V2:V9)</f>
         <v>0</v>
       </c>
-      <c r="W12" s="0" t="n">
+      <c r="W13" s="0" t="n">
         <f aca="false">SUM(W2:W9)</f>
         <v>0</v>
       </c>
@@ -5879,9 +6025,9 @@
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
created two new modules nfcaccess and codeaccess, added abstract foundation to nfcaccess module, moved prompts to a seperate module called prompts, updated scrum tables
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
   <si>
     <t>New estimates of effort remaining as of sprint</t>
   </si>
@@ -204,7 +204,7 @@
     <t>Napraviti logiku dodavanja u grupu na mobilnom uređaju</t>
   </si>
   <si>
-    <t>Napraviti module za dodavanje u grupu</t>
+    <t>Napraviti modul za dodavanje u grupu kodom (codeaccess)</t>
   </si>
   <si>
     <t>Napraviti logiku web servisa za dodavanje ljudi u grupu</t>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>NFC beam aktivnost (UI)</t>
+  </si>
+  <si>
+    <t>Napraviti NFC apstraktne temelje</t>
+  </si>
+  <si>
+    <t>Dodati gumbe za pokretanje NFC beam aktivnosti</t>
   </si>
   <si>
     <t>Napraviti animaciju za NFC beam</t>
@@ -507,7 +513,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -680,10 +686,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1162,11 +1164,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="11239909"/>
-        <c:axId val="56335224"/>
+        <c:axId val="94515400"/>
+        <c:axId val="88664495"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="11239909"/>
+        <c:axId val="94515400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1206,14 +1208,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="56335224"/>
+        <c:crossAx val="88664495"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56335224"/>
+        <c:axId val="88664495"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,7 +1265,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="11239909"/>
+        <c:crossAx val="94515400"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1673,11 +1675,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="73296840"/>
-        <c:axId val="45880741"/>
+        <c:axId val="94962230"/>
+        <c:axId val="25527226"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73296840"/>
+        <c:axId val="94962230"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,14 +1695,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="45880741"/>
+        <c:crossAx val="25527226"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45880741"/>
+        <c:axId val="25527226"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1725,7 +1727,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="73296840"/>
+        <c:crossAx val="94962230"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1814,7 +1816,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1987,7 +1989,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="5"/>
+            <c:size val="4"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -2135,11 +2137,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="5998308"/>
-        <c:axId val="72652294"/>
+        <c:axId val="78459777"/>
+        <c:axId val="74287243"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="5998308"/>
+        <c:axId val="78459777"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2155,14 +2157,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="72652294"/>
+        <c:crossAx val="74287243"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72652294"/>
+        <c:axId val="74287243"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2187,7 +2189,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="5998308"/>
+        <c:crossAx val="78459777"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2227,15 +2229,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2234160</xdr:colOff>
+      <xdr:colOff>2261160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>88200</xdr:rowOff>
+      <xdr:rowOff>79200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1223640</xdr:colOff>
+      <xdr:colOff>1250280</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>186120</xdr:rowOff>
+      <xdr:rowOff>176760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2243,8 +2245,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2234160" y="7138440"/>
-        <a:ext cx="9964080" cy="5622480"/>
+        <a:off x="2261160" y="7129440"/>
+        <a:ext cx="9963720" cy="5622120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2262,15 +2264,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>87120</xdr:colOff>
+      <xdr:colOff>114120</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>290520</xdr:rowOff>
+      <xdr:rowOff>281520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>688320</xdr:colOff>
+      <xdr:colOff>714960</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>34560</xdr:rowOff>
+      <xdr:rowOff>25200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2278,8 +2280,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2596320" y="7066440"/>
-        <a:ext cx="9043200" cy="4305240"/>
+        <a:off x="2623320" y="7057440"/>
+        <a:ext cx="9042840" cy="4304880"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2297,15 +2299,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>90360</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>18000</xdr:rowOff>
+      <xdr:colOff>117360</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>699480</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>6120</xdr:rowOff>
+      <xdr:colOff>726120</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2313,8 +2315,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4056480" y="5552640"/>
-        <a:ext cx="5758920" cy="3239280"/>
+        <a:off x="4083480" y="6696720"/>
+        <a:ext cx="5758560" cy="3239280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2335,7 +2337,7 @@
   <dimension ref="A1:I65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2618,7 +2620,7 @@
   <dimension ref="A1:B65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5211,10 +5213,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AN13"/>
+  <dimension ref="A1:AR15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N28" activeCellId="0" sqref="N28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -5319,28 +5321,32 @@
         <v>23</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E2" s="23" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F2" s="23" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G2" s="23" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H2" s="29" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I2" s="29" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="J2" s="29" t="n">
-        <v>6</v>
-      </c>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
+        <v>2</v>
+      </c>
+      <c r="K2" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2" s="29" t="n">
+        <v>2</v>
+      </c>
       <c r="M2" s="29"/>
       <c r="N2" s="29"/>
       <c r="O2" s="29"/>
@@ -5382,8 +5388,12 @@
       <c r="J3" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
+      <c r="K3" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" s="25" t="n">
+        <v>3</v>
+      </c>
       <c r="M3" s="25"/>
       <c r="N3" s="25"/>
       <c r="O3" s="25"/>
@@ -5405,28 +5415,32 @@
         <v>23</v>
       </c>
       <c r="D4" s="38" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E4" s="38" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F4" s="38" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G4" s="38" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H4" s="25" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I4" s="25" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J4" s="25" t="n">
-        <v>5</v>
-      </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
+        <v>2</v>
+      </c>
+      <c r="K4" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" s="25" t="n">
+        <v>2</v>
+      </c>
       <c r="M4" s="24"/>
       <c r="N4" s="24"/>
       <c r="O4" s="24"/>
@@ -5441,14 +5455,14 @@
     </row>
     <row r="5" customFormat="false" ht="25.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20"/>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" s="21" t="n">
         <v>0</v>
@@ -5518,28 +5532,32 @@
         <v>23</v>
       </c>
       <c r="D6" s="6" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6" s="23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F6" s="23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G6" s="23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H6" s="23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I6" s="23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J6" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="K6" s="21"/>
-      <c r="L6" s="21"/>
+        <v>2</v>
+      </c>
+      <c r="K6" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" s="23" t="n">
+        <v>2</v>
+      </c>
       <c r="M6" s="21"/>
       <c r="N6" s="21"/>
       <c r="O6" s="21"/>
@@ -5554,7 +5572,7 @@
     </row>
     <row r="7" customFormat="false" ht="25.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20"/>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="21" t="s">
         <v>65</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -5624,29 +5642,29 @@
     </row>
     <row r="8" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="20"/>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="26" t="s">
         <v>66</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D8" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" s="23" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F8" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G8" s="6" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H8" s="0" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I8" s="25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J8" s="24" t="n">
         <v>0</v>
@@ -5695,7 +5713,7 @@
       <c r="A9" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="43" t="s">
         <v>68</v>
       </c>
       <c r="C9" s="33" t="s">
@@ -5722,8 +5740,12 @@
       <c r="J9" s="34" t="n">
         <v>2</v>
       </c>
-      <c r="K9" s="35"/>
-      <c r="L9" s="34"/>
+      <c r="K9" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="L9" s="34" t="n">
+        <v>2</v>
+      </c>
       <c r="M9" s="34"/>
       <c r="N9" s="34"/>
       <c r="O9" s="34"/>
@@ -5738,7 +5760,7 @@
     </row>
     <row r="10" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20"/>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="37" t="s">
         <v>69</v>
       </c>
       <c r="C10" s="38" t="s">
@@ -5765,8 +5787,8 @@
       <c r="J10" s="39" t="n">
         <v>2</v>
       </c>
-      <c r="K10" s="24" t="n">
-        <v>0</v>
+      <c r="K10" s="28" t="n">
+        <v>2</v>
       </c>
       <c r="L10" s="24" t="n">
         <v>0</v>
@@ -5804,230 +5826,392 @@
       <c r="W10" s="24" t="n">
         <v>0</v>
       </c>
+      <c r="X10" s="38"/>
+      <c r="Y10" s="38"/>
+      <c r="Z10" s="38"/>
+      <c r="AA10" s="38"/>
+      <c r="AB10" s="38"/>
+      <c r="AC10" s="39"/>
+      <c r="AD10" s="39"/>
+      <c r="AE10" s="39"/>
+      <c r="AF10" s="28"/>
+      <c r="AG10" s="39"/>
+      <c r="AH10" s="39"/>
+      <c r="AI10" s="39"/>
+      <c r="AJ10" s="39"/>
+      <c r="AK10" s="39"/>
+      <c r="AL10" s="39"/>
+      <c r="AM10" s="39"/>
+      <c r="AN10" s="39"/>
+      <c r="AO10" s="39"/>
+      <c r="AP10" s="39"/>
+      <c r="AQ10" s="28"/>
+      <c r="AR10" s="40"/>
     </row>
     <row r="11" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
-      <c r="B11" s="46" t="s">
+      <c r="B11" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="47" t="s">
+      <c r="C11" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="47" t="n">
-        <v>4</v>
-      </c>
-      <c r="E11" s="47" t="n">
-        <v>4</v>
-      </c>
-      <c r="F11" s="47" t="n">
-        <v>4</v>
-      </c>
-      <c r="G11" s="47" t="n">
-        <v>4</v>
-      </c>
-      <c r="H11" s="48" t="n">
-        <v>4</v>
-      </c>
-      <c r="I11" s="48" t="n">
-        <v>4</v>
-      </c>
-      <c r="J11" s="48" t="n">
-        <v>4</v>
-      </c>
-      <c r="K11" s="49"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
-      <c r="N11" s="48"/>
-      <c r="O11" s="48"/>
-      <c r="P11" s="48"/>
-      <c r="Q11" s="48"/>
-      <c r="R11" s="48"/>
-      <c r="S11" s="48"/>
-      <c r="T11" s="48"/>
-      <c r="U11" s="48"/>
-      <c r="V11" s="49"/>
-      <c r="W11" s="50"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="41" t="s">
+      <c r="D11" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="28" t="n">
+        <v>2</v>
+      </c>
+      <c r="L11" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
+      <c r="P11" s="24"/>
+      <c r="Q11" s="24"/>
+      <c r="R11" s="24"/>
+      <c r="S11" s="24"/>
+      <c r="T11" s="24"/>
+      <c r="U11" s="24"/>
+      <c r="V11" s="24"/>
+      <c r="W11" s="24"/>
+      <c r="X11" s="38"/>
+      <c r="Y11" s="38"/>
+      <c r="Z11" s="38"/>
+      <c r="AA11" s="38"/>
+      <c r="AB11" s="38"/>
+      <c r="AC11" s="39"/>
+      <c r="AD11" s="39"/>
+      <c r="AE11" s="39"/>
+      <c r="AF11" s="28"/>
+      <c r="AG11" s="39"/>
+      <c r="AH11" s="39"/>
+      <c r="AI11" s="39"/>
+      <c r="AJ11" s="39"/>
+      <c r="AK11" s="39"/>
+      <c r="AL11" s="39"/>
+      <c r="AM11" s="39"/>
+      <c r="AN11" s="39"/>
+      <c r="AO11" s="39"/>
+      <c r="AP11" s="39"/>
+      <c r="AQ11" s="28"/>
+      <c r="AR11" s="40"/>
+    </row>
+    <row r="12" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="20"/>
+      <c r="B12" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="20"/>
+      <c r="B13" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="46" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" s="46" t="n">
+        <v>2</v>
+      </c>
+      <c r="F13" s="46" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="46" t="n">
+        <v>2</v>
+      </c>
+      <c r="H13" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" s="48" t="n">
+        <v>2</v>
+      </c>
+      <c r="L13" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="M13" s="47"/>
+      <c r="N13" s="47"/>
+      <c r="O13" s="47"/>
+      <c r="P13" s="47"/>
+      <c r="Q13" s="47"/>
+      <c r="R13" s="47"/>
+      <c r="S13" s="47"/>
+      <c r="T13" s="47"/>
+      <c r="U13" s="47"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="49"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="0" t="n">
-        <f aca="false">SUM(D2:D9)</f>
-        <v>29</v>
-      </c>
-      <c r="E12" s="42" t="n">
-        <f aca="false">D12-($D$12/19)</f>
-        <v>27.4736842105263</v>
-      </c>
-      <c r="F12" s="42" t="n">
-        <f aca="false">E12-($D$12/19)</f>
-        <v>25.9473684210526</v>
-      </c>
-      <c r="G12" s="42" t="n">
-        <f aca="false">F12-($D$12/19)</f>
-        <v>24.4210526315789</v>
-      </c>
-      <c r="H12" s="42" t="n">
-        <f aca="false">G12-($D$12/19)</f>
-        <v>22.8947368421053</v>
-      </c>
-      <c r="I12" s="42" t="n">
-        <f aca="false">H12-($D$12/19)</f>
-        <v>21.3684210526316</v>
-      </c>
-      <c r="J12" s="42" t="n">
-        <f aca="false">I12-($D$12/19)</f>
-        <v>19.8421052631579</v>
-      </c>
-      <c r="K12" s="42" t="n">
-        <f aca="false">J12-($D$12/19)</f>
-        <v>18.3157894736842</v>
-      </c>
-      <c r="L12" s="42" t="n">
-        <f aca="false">K12-($D$12/19)</f>
-        <v>16.7894736842105</v>
-      </c>
-      <c r="M12" s="42" t="n">
-        <f aca="false">L12-($D$12/19)</f>
-        <v>15.2631578947368</v>
-      </c>
-      <c r="N12" s="42" t="n">
-        <f aca="false">M12-($D$12/19)</f>
-        <v>13.7368421052632</v>
-      </c>
-      <c r="O12" s="42" t="n">
-        <f aca="false">N12-($D$12/19)</f>
-        <v>12.2105263157895</v>
-      </c>
-      <c r="P12" s="42" t="n">
-        <f aca="false">O12-($D$12/19)</f>
-        <v>10.6842105263158</v>
-      </c>
-      <c r="Q12" s="42" t="n">
-        <f aca="false">P12-($D$12/19)</f>
-        <v>9.1578947368421</v>
-      </c>
-      <c r="R12" s="42" t="n">
-        <f aca="false">Q12-($D$12/19)</f>
-        <v>7.63157894736841</v>
-      </c>
-      <c r="S12" s="42" t="n">
-        <f aca="false">R12-($D$12/19)</f>
-        <v>6.10526315789473</v>
-      </c>
-      <c r="T12" s="42" t="n">
-        <f aca="false">S12-($D$12/19)</f>
-        <v>4.57894736842104</v>
-      </c>
-      <c r="U12" s="42" t="n">
-        <f aca="false">T12-($D$12/19)</f>
-        <v>3.05263157894736</v>
-      </c>
-      <c r="V12" s="42" t="n">
-        <f aca="false">U12-($D$12/19)</f>
-        <v>1.52631578947368</v>
-      </c>
-      <c r="W12" s="42" t="n">
-        <f aca="false">V12-($D$12/19)</f>
-        <v>-9.32587340685132E-015</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="41" t="s">
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="0" t="n">
+        <f aca="false">SUM(D2:D13)</f>
+        <v>24</v>
+      </c>
+      <c r="E14" s="42" t="n">
+        <f aca="false">D14-($D$14/19)</f>
+        <v>22.7368421052632</v>
+      </c>
+      <c r="F14" s="42" t="n">
+        <f aca="false">E14-($D$14/19)</f>
+        <v>21.4736842105263</v>
+      </c>
+      <c r="G14" s="42" t="n">
+        <f aca="false">F14-($D$14/19)</f>
+        <v>20.2105263157895</v>
+      </c>
+      <c r="H14" s="42" t="n">
+        <f aca="false">G14-($D$14/19)</f>
+        <v>18.9473684210526</v>
+      </c>
+      <c r="I14" s="42" t="n">
+        <f aca="false">H14-($D$14/19)</f>
+        <v>17.6842105263158</v>
+      </c>
+      <c r="J14" s="42" t="n">
+        <f aca="false">I14-($D$14/19)</f>
+        <v>16.4210526315789</v>
+      </c>
+      <c r="K14" s="42" t="n">
+        <f aca="false">J14-($D$14/19)</f>
+        <v>15.1578947368421</v>
+      </c>
+      <c r="L14" s="42" t="n">
+        <f aca="false">K14-($D$14/19)</f>
+        <v>13.8947368421053</v>
+      </c>
+      <c r="M14" s="42" t="n">
+        <f aca="false">L14-($D$14/19)</f>
+        <v>12.6315789473684</v>
+      </c>
+      <c r="N14" s="42" t="n">
+        <f aca="false">M14-($D$14/19)</f>
+        <v>11.3684210526316</v>
+      </c>
+      <c r="O14" s="42" t="n">
+        <f aca="false">N14-($D$14/19)</f>
+        <v>10.1052631578947</v>
+      </c>
+      <c r="P14" s="42" t="n">
+        <f aca="false">O14-($D$14/19)</f>
+        <v>8.84210526315789</v>
+      </c>
+      <c r="Q14" s="42" t="n">
+        <f aca="false">P14-($D$14/19)</f>
+        <v>7.57894736842105</v>
+      </c>
+      <c r="R14" s="42" t="n">
+        <f aca="false">Q14-($D$14/19)</f>
+        <v>6.31578947368421</v>
+      </c>
+      <c r="S14" s="42" t="n">
+        <f aca="false">R14-($D$14/19)</f>
+        <v>5.05263157894736</v>
+      </c>
+      <c r="T14" s="42" t="n">
+        <f aca="false">S14-($D$14/19)</f>
+        <v>3.78947368421052</v>
+      </c>
+      <c r="U14" s="42" t="n">
+        <f aca="false">T14-($D$14/19)</f>
+        <v>2.52631578947368</v>
+      </c>
+      <c r="V14" s="42" t="n">
+        <f aca="false">U14-($D$14/19)</f>
+        <v>1.26315789473684</v>
+      </c>
+      <c r="W14" s="42" t="n">
+        <f aca="false">V14-($D$14/19)</f>
+        <v>-5.32907051820075E-015</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="0" t="n">
-        <f aca="false">SUM(D2:D9)</f>
-        <v>29</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <f aca="false">SUM(E2:E9)</f>
-        <v>23</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <f aca="false">SUM(F2:F9)</f>
-        <v>23</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <f aca="false">SUM(G2:G9)</f>
-        <v>23</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <f aca="false">SUM(H2:H9)</f>
-        <v>23</v>
-      </c>
-      <c r="I13" s="0" t="n">
-        <f aca="false">SUM(I2:I9)</f>
-        <v>23</v>
-      </c>
-      <c r="J13" s="0" t="n">
-        <f aca="false">SUM(J2:J9)</f>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="0" t="n">
+        <f aca="false">SUM(D2:D13)</f>
+        <v>24</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <f aca="false">SUM(E2:E13)</f>
+        <v>20</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <f aca="false">SUM(F2:F13)</f>
+        <v>20</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">SUM(G2:G13)</f>
+        <v>20</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">SUM(H2:H13)</f>
+        <v>20</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">SUM(I2:I13)</f>
+        <v>20</v>
+      </c>
+      <c r="J15" s="0" t="n">
+        <f aca="false">SUM(J2:J13)</f>
         <v>19</v>
       </c>
-      <c r="K13" s="0" t="n">
-        <f aca="false">SUM(K2:K9)</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="0" t="n">
-        <f aca="false">SUM(L2:L9)</f>
-        <v>0</v>
-      </c>
-      <c r="M13" s="0" t="n">
-        <f aca="false">SUM(M2:M9)</f>
-        <v>0</v>
-      </c>
-      <c r="N13" s="0" t="n">
-        <f aca="false">SUM(N2:N9)</f>
-        <v>0</v>
-      </c>
-      <c r="O13" s="0" t="n">
-        <f aca="false">SUM(O2:O9)</f>
-        <v>0</v>
-      </c>
-      <c r="P13" s="0" t="n">
-        <f aca="false">SUM(P2:P9)</f>
-        <v>0</v>
-      </c>
-      <c r="Q13" s="0" t="n">
-        <f aca="false">SUM(Q2:Q9)</f>
-        <v>0</v>
-      </c>
-      <c r="R13" s="0" t="n">
-        <f aca="false">SUM(R2:R9)</f>
-        <v>0</v>
-      </c>
-      <c r="S13" s="0" t="n">
-        <f aca="false">SUM(S2:S9)</f>
-        <v>0</v>
-      </c>
-      <c r="T13" s="0" t="n">
-        <f aca="false">SUM(T2:T9)</f>
-        <v>0</v>
-      </c>
-      <c r="U13" s="0" t="n">
-        <f aca="false">SUM(U2:U9)</f>
-        <v>0</v>
-      </c>
-      <c r="V13" s="0" t="n">
-        <f aca="false">SUM(V2:V9)</f>
-        <v>0</v>
-      </c>
-      <c r="W13" s="0" t="n">
-        <f aca="false">SUM(W2:W9)</f>
+      <c r="K15" s="0" t="n">
+        <f aca="false">SUM(K2:K13)</f>
+        <v>17</v>
+      </c>
+      <c r="L15" s="0" t="n">
+        <f aca="false">SUM(L2:L13)</f>
+        <v>15</v>
+      </c>
+      <c r="M15" s="0" t="n">
+        <f aca="false">SUM(M2:M13)</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="0" t="n">
+        <f aca="false">SUM(N2:N13)</f>
+        <v>0</v>
+      </c>
+      <c r="O15" s="0" t="n">
+        <f aca="false">SUM(O2:O13)</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="0" t="n">
+        <f aca="false">SUM(P2:P13)</f>
+        <v>0</v>
+      </c>
+      <c r="Q15" s="0" t="n">
+        <f aca="false">SUM(Q2:Q13)</f>
+        <v>0</v>
+      </c>
+      <c r="R15" s="0" t="n">
+        <f aca="false">SUM(R2:R13)</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="0" t="n">
+        <f aca="false">SUM(S2:S13)</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="0" t="n">
+        <f aca="false">SUM(T2:T13)</f>
+        <v>0</v>
+      </c>
+      <c r="U15" s="0" t="n">
+        <f aca="false">SUM(U2:U13)</f>
+        <v>0</v>
+      </c>
+      <c r="V15" s="0" t="n">
+        <f aca="false">SUM(V2:V13)</f>
+        <v>0</v>
+      </c>
+      <c r="W15" s="0" t="n">
+        <f aca="false">SUM(W2:W13)</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
ispravci i dodana dretva
</commit_message>
<xml_diff>
--- a/dokumentacija/air scrum tablice.xlsx
+++ b/dokumentacija/air scrum tablice.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="72">
   <si>
     <t>New estimates of effort remaining as of sprint</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>Napraviti logiku dodavanja u grupu na mobilnom uređaju</t>
-  </si>
-  <si>
-    <t>Napraviti modul za dodavanje u grupu kodom (codeaccess)</t>
   </si>
   <si>
     <t>Napraviti logiku web servisa za dodavanje ljudi u grupu</t>
@@ -249,13 +246,12 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="10"/>
@@ -277,14 +273,12 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
       <b val="true"/>
@@ -292,22 +286,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -330,6 +308,11 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="13"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="13"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -513,7 +496,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="45">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -618,31 +601,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -654,15 +621,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -674,10 +641,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -686,15 +649,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -706,11 +669,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -822,7 +785,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ideal</c:f>
+              <c:f>label 0</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -854,75 +817,75 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 backlog'!$D$2:$W$2</c:f>
+              <c:f>categories</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Initial estimate of effort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10/20/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10/21/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10/22/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10/23/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10/24/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10/25/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10/26/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10/27/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10/28/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10/29/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10/30/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10/31/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11/1/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11/2/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11/3/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11/4/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11/5/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11/6/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11/7/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 backlog'!$D$18:$W$18</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -995,7 +958,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>current</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1027,75 +990,75 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 1 backlog'!$D$2:$W$2</c:f>
+              <c:f>categories</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Initial estimate of effort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10/20/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10/21/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10/22/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10/23/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10/24/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10/25/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10/26/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10/27/2015</c:v>
+                  <c:v>42300</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10/28/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10/29/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10/30/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10/31/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11/1/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11/2/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11/3/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11/4/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11/5/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11/6/2015</c:v>
+                  <c:v>42310</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11/7/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 1 backlog'!$D$19:$W$19</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1164,11 +1127,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="5695082"/>
-        <c:axId val="10400345"/>
+        <c:axId val="30312943"/>
+        <c:axId val="55405521"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="5695082"/>
+        <c:axId val="30312943"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1208,14 +1171,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="10400345"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="55405521"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10400345"/>
+        <c:axId val="55405521"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1265,7 +1228,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="5695082"/>
+        <c:crossAx val="30312943"/>
         <c:crossesAt val="1"/>
       </c:valAx>
       <c:spPr>
@@ -1333,7 +1296,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>ideal</c:f>
+              <c:f>label 0</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1365,75 +1328,75 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 2 backlog'!$D$2:$W$2</c:f>
+              <c:f>categories</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Initial estimate of effort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11/9/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11/10/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11/11/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11/12/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11/13/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11/14/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11/15/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11/16/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11/17/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11/18/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11/19/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11/20/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11/21/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11/22/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11/23/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11/24/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11/25/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11/26/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11/27/2015</c:v>
+                  <c:v>42340</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2 backlog'!$D$15:$W$15</c:f>
+              <c:f>0</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1506,7 +1469,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>current</c:f>
+              <c:f>label 1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1538,75 +1501,75 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Sprint 2 backlog'!$D$2:$W$2</c:f>
+              <c:f>categories</c:f>
               <c:strCache>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>Initial estimate of effort</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11/9/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11/10/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11/11/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11/12/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11/13/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11/14/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11/15/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11/16/2015</c:v>
+                  <c:v>42320</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11/17/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11/18/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11/19/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>11/20/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11/21/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>11/22/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11/23/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>11/24/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11/25/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11/26/2015</c:v>
+                  <c:v>42330</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11/27/2015</c:v>
+                  <c:v>42340</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Sprint 2 backlog'!$D$16:$W$16</c:f>
+              <c:f>1</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1620,52 +1583,52 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="19">
                   <c:v>0</c:v>
@@ -1675,11 +1638,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84867747"/>
-        <c:axId val="11392203"/>
+        <c:axId val="85113675"/>
+        <c:axId val="37223111"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84867747"/>
+        <c:axId val="85113675"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1695,14 +1658,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="11392203"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="37223111"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11392203"/>
+        <c:axId val="37223111"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1690,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84867747"/>
+        <c:crossAx val="85113675"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -1776,7 +1739,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr b="1" sz="1300">
+              <a:rPr sz="1300">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Burndown chart</a:t>
@@ -1816,7 +1779,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="7"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -1900,64 +1863,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.1578947368421</c:v>
+                  <c:v>22.7368421052632</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>31.3157894736842</c:v>
+                  <c:v>21.4736842105263</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.4736842105263</c:v>
+                  <c:v>20.2105263157895</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27.6315789473684</c:v>
+                  <c:v>18.9473684210526</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.7894736842105</c:v>
+                  <c:v>17.6842105263158</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.9473684210526</c:v>
+                  <c:v>16.4210526315789</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.1052631578947</c:v>
+                  <c:v>15.1578947368421</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.2631578947368</c:v>
+                  <c:v>13.8947368421053</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.421052631579</c:v>
+                  <c:v>12.6315789473684</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.5789473684211</c:v>
+                  <c:v>11.3684210526316</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14.7368421052632</c:v>
+                  <c:v>10.1052631578947</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.8947368421053</c:v>
+                  <c:v>8.84210526315789</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.0526315789474</c:v>
+                  <c:v>7.57894736842105</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9.21052631578948</c:v>
+                  <c:v>6.31578947368421</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.36842105263159</c:v>
+                  <c:v>5.05263157894736</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.52631578947369</c:v>
+                  <c:v>3.78947368421052</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.6842105263158</c:v>
+                  <c:v>2.52631578947368</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.8421052631579</c:v>
+                  <c:v>1.26315789473684</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9.76996261670138E-015</c:v>
+                  <c:v>-5.32907051820075E-015</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1989,7 +1952,7 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:size val="3"/>
+            <c:size val="7"/>
           </c:marker>
           <c:dLbls>
             <c:showLegendKey val="0"/>
@@ -2073,75 +2036,75 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>35</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="8231586"/>
-        <c:axId val="23543265"/>
+        <c:axId val="87839364"/>
+        <c:axId val="18779672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8231586"/>
+        <c:axId val="87839364"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2157,14 +2120,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="23543265"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="18779672"/>
+        <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23543265"/>
+        <c:axId val="18779672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2189,7 +2152,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="8231586"/>
+        <c:crossAx val="87839364"/>
         <c:crossesAt val="0"/>
       </c:valAx>
       <c:spPr>
@@ -2229,15 +2192,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>2288160</xdr:colOff>
+      <xdr:colOff>2315160</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>70200</xdr:rowOff>
+      <xdr:rowOff>61200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1276920</xdr:colOff>
+      <xdr:colOff>1303560</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>167400</xdr:rowOff>
+      <xdr:rowOff>158040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2245,8 +2208,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2288160" y="7120440"/>
-        <a:ext cx="9963360" cy="5621760"/>
+        <a:off x="2315160" y="7111440"/>
+        <a:ext cx="9963000" cy="5621400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2264,15 +2227,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>141120</xdr:colOff>
+      <xdr:colOff>168840</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>272520</xdr:rowOff>
+      <xdr:rowOff>263520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>741600</xdr:colOff>
+      <xdr:colOff>768240</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>15840</xdr:rowOff>
+      <xdr:rowOff>6480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2280,8 +2243,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="2650320" y="7048440"/>
-        <a:ext cx="9042480" cy="4304520"/>
+        <a:off x="2678040" y="7039440"/>
+        <a:ext cx="9041400" cy="4304160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2299,15 +2262,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>144360</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>105480</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>135720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>752760</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>150480</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>183960</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>126360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2315,8 +2278,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4110480" y="6687720"/>
-        <a:ext cx="5758200" cy="3238920"/>
+        <a:off x="4494600" y="5913360"/>
+        <a:ext cx="8479440" cy="4542480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2337,7 +2300,7 @@
   <dimension ref="A1:I65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="1" sqref="O8:W8 G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2620,7 +2583,7 @@
   <dimension ref="A1:B65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A48" activeCellId="0" sqref="A48"/>
+      <selection pane="topLeft" activeCell="A48" activeCellId="1" sqref="O8:W8 A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2718,8 +2681,8 @@
   </sheetPr>
   <dimension ref="A1:X19"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="W9" activeCellId="0" sqref="W9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W9" activeCellId="1" sqref="O8:W8 W9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3248,7 +3211,7 @@
     </row>
     <row r="9" customFormat="false" ht="30.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="20"/>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="21" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="6" t="s">
@@ -3318,7 +3281,7 @@
     </row>
     <row r="10" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20"/>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -3345,7 +3308,7 @@
       <c r="J10" s="25" t="n">
         <v>4</v>
       </c>
-      <c r="K10" s="28" t="n">
+      <c r="K10" s="25" t="n">
         <v>2</v>
       </c>
       <c r="L10" s="0" t="n">
@@ -3477,13 +3440,13 @@
       <c r="H12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I12" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="J12" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="K12" s="30" t="n">
+      <c r="I12" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" s="27" t="n">
         <v>2</v>
       </c>
       <c r="L12" s="0" t="n">
@@ -3492,7 +3455,7 @@
       <c r="M12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="N12" s="29" t="n">
+      <c r="N12" s="27" t="n">
         <v>1</v>
       </c>
       <c r="O12" s="0" t="n">
@@ -3525,7 +3488,7 @@
     </row>
     <row r="13" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="21" t="s">
         <v>38</v>
       </c>
       <c r="C13" s="6" t="s">
@@ -3546,13 +3509,13 @@
       <c r="H13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="I13" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="J13" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="K13" s="30" t="n">
+      <c r="I13" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="J13" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="K13" s="27" t="n">
         <v>2</v>
       </c>
       <c r="L13" s="0" t="n">
@@ -3561,7 +3524,7 @@
       <c r="M13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="N13" s="29" t="n">
+      <c r="N13" s="27" t="n">
         <v>2</v>
       </c>
       <c r="O13" s="0" t="n">
@@ -3588,7 +3551,7 @@
       <c r="V13" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="W13" s="31" t="n">
+      <c r="W13" s="22" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3665,94 +3628,94 @@
       <c r="A15" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D15" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="E15" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="H15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="I15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="J15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="K15" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="L15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="M15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="N15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="O15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="P15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="R15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="S15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="T15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="U15" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="V15" s="36" t="n">
-        <v>0</v>
-      </c>
-      <c r="W15" s="36" t="n">
+      <c r="D15" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="J15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="K15" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="L15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="M15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="N15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="O15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="P15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="R15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="S15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="T15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="U15" s="30" t="n">
+        <v>3</v>
+      </c>
+      <c r="V15" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W15" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="20"/>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="33" t="s">
         <v>42</v>
       </c>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="E16" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="F16" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="G16" s="38" t="n">
-        <v>3</v>
-      </c>
-      <c r="H16" s="39" t="n">
+      <c r="D16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="E16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="F16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="G16" s="34" t="n">
+        <v>3</v>
+      </c>
+      <c r="H16" s="35" t="n">
         <v>3</v>
       </c>
       <c r="I16" s="25" t="n">
@@ -3761,67 +3724,67 @@
       <c r="J16" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="K16" s="28" t="n">
-        <v>3</v>
-      </c>
-      <c r="L16" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="M16" s="39" t="n">
+      <c r="K16" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="L16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="M16" s="35" t="n">
         <v>3</v>
       </c>
       <c r="N16" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="O16" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="P16" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q16" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="R16" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="S16" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="T16" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="U16" s="39" t="n">
-        <v>3</v>
-      </c>
-      <c r="V16" s="40" t="n">
-        <v>0</v>
-      </c>
-      <c r="W16" s="40" t="n">
+      <c r="O16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="P16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="R16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="S16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="T16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="U16" s="35" t="n">
+        <v>3</v>
+      </c>
+      <c r="V16" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W16" s="24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="20"/>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="F17" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H17" s="39" t="n">
+      <c r="D17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="35" t="n">
         <v>1</v>
       </c>
       <c r="I17" s="25" t="n">
@@ -3830,13 +3793,13 @@
       <c r="J17" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K17" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="L17" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="M17" s="39" t="n">
+      <c r="K17" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L17" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M17" s="35" t="n">
         <v>1</v>
       </c>
       <c r="N17" s="24" t="n">
@@ -3871,98 +3834,98 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="33" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
       <c r="D18" s="0" t="n">
         <f aca="false">SUM(D3:D17)</f>
         <v>30</v>
       </c>
-      <c r="E18" s="42" t="n">
+      <c r="E18" s="37" t="n">
         <f aca="false">D18-($D$18/19)</f>
         <v>28.4210526315789</v>
       </c>
-      <c r="F18" s="42" t="n">
+      <c r="F18" s="37" t="n">
         <f aca="false">E18-($D$18/19)</f>
         <v>26.8421052631579</v>
       </c>
-      <c r="G18" s="42" t="n">
+      <c r="G18" s="37" t="n">
         <f aca="false">F18-($D$18/19)</f>
         <v>25.2631578947368</v>
       </c>
-      <c r="H18" s="42" t="n">
+      <c r="H18" s="37" t="n">
         <f aca="false">G18-($D$18/19)</f>
         <v>23.6842105263158</v>
       </c>
-      <c r="I18" s="42" t="n">
+      <c r="I18" s="37" t="n">
         <f aca="false">H18-($D$18/19)</f>
         <v>22.1052631578947</v>
       </c>
-      <c r="J18" s="42" t="n">
+      <c r="J18" s="37" t="n">
         <f aca="false">I18-($D$18/19)</f>
         <v>20.5263157894737</v>
       </c>
-      <c r="K18" s="42" t="n">
+      <c r="K18" s="37" t="n">
         <f aca="false">J18-($D$18/19)</f>
         <v>18.9473684210526</v>
       </c>
-      <c r="L18" s="42" t="n">
+      <c r="L18" s="37" t="n">
         <f aca="false">K18-($D$18/19)</f>
         <v>17.3684210526316</v>
       </c>
-      <c r="M18" s="42" t="n">
+      <c r="M18" s="37" t="n">
         <f aca="false">L18-($D$18/19)</f>
         <v>15.7894736842105</v>
       </c>
-      <c r="N18" s="42" t="n">
+      <c r="N18" s="37" t="n">
         <f aca="false">M18-($D$18/19)</f>
         <v>14.2105263157895</v>
       </c>
-      <c r="O18" s="42" t="n">
+      <c r="O18" s="37" t="n">
         <f aca="false">N18-($D$18/19)</f>
         <v>12.6315789473684</v>
       </c>
-      <c r="P18" s="42" t="n">
+      <c r="P18" s="37" t="n">
         <f aca="false">O18-($D$18/19)</f>
         <v>11.0526315789474</v>
       </c>
-      <c r="Q18" s="42" t="n">
+      <c r="Q18" s="37" t="n">
         <f aca="false">P18-($D$18/19)</f>
         <v>9.47368421052632</v>
       </c>
-      <c r="R18" s="42" t="n">
+      <c r="R18" s="37" t="n">
         <f aca="false">Q18-($D$18/19)</f>
         <v>7.89473684210527</v>
       </c>
-      <c r="S18" s="42" t="n">
+      <c r="S18" s="37" t="n">
         <f aca="false">R18-($D$18/19)</f>
         <v>6.31578947368422</v>
       </c>
-      <c r="T18" s="42" t="n">
+      <c r="T18" s="37" t="n">
         <f aca="false">S18-($D$18/19)</f>
         <v>4.73684210526316</v>
       </c>
-      <c r="U18" s="42" t="n">
+      <c r="U18" s="37" t="n">
         <f aca="false">T18-($D$18/19)</f>
         <v>3.15789473684211</v>
       </c>
-      <c r="V18" s="42" t="n">
+      <c r="V18" s="37" t="n">
         <f aca="false">U18-($D$18/19)</f>
         <v>1.57894736842106</v>
       </c>
-      <c r="W18" s="42" t="n">
+      <c r="W18" s="37" t="n">
         <f aca="false">V18-($D$18/19)</f>
         <v>6.66133814775094E-015</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="30.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
       <c r="D19" s="0" t="n">
         <f aca="false">SUM(D3:D17)</f>
         <v>30</v>
@@ -4071,7 +4034,7 @@
   <dimension ref="A1:W17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P11" activeCellId="0" sqref="P11"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="O8:W8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4204,49 +4167,49 @@
       <c r="G3" s="23" t="n">
         <v>3</v>
       </c>
-      <c r="H3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="I3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="K3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="L3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="M3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="N3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="O3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="P3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="R3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="S3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="T3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="U3" s="29" t="n">
-        <v>3</v>
-      </c>
-      <c r="V3" s="29" t="n">
+      <c r="H3" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="J3" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="K3" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="L3" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="N3" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="O3" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="R3" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="S3" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="T3" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="U3" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" s="27" t="n">
         <v>1</v>
       </c>
       <c r="W3" s="22" t="n">
@@ -4342,50 +4305,50 @@
       <c r="G5" s="23" t="n">
         <v>1</v>
       </c>
-      <c r="H5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="P5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="R5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="S5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="T5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="U5" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="V5" s="29" t="n">
-        <v>1</v>
+      <c r="H5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="22" t="n">
+        <v>0</v>
       </c>
       <c r="W5" s="22" t="n">
         <v>0</v>
@@ -4418,37 +4381,37 @@
         <v>3</v>
       </c>
       <c r="J6" s="25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K6" s="25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6" s="25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M6" s="25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N6" s="25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O6" s="25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P6" s="25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Q6" s="25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="R6" s="25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S6" s="25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="T6" s="25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="U6" s="24" t="n">
         <v>0</v>
@@ -4505,25 +4468,25 @@
         <v>4</v>
       </c>
       <c r="P7" s="25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="Q7" s="25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="R7" s="25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S7" s="25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T7" s="25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U7" s="25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V7" s="25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="W7" s="24" t="n">
         <v>0</v>
@@ -4715,22 +4678,22 @@
         <v>4</v>
       </c>
       <c r="Q10" s="25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R10" s="25" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S10" s="25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="T10" s="25" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="U10" s="25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V10" s="25" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="W10" s="24" t="n">
         <v>0</v>
@@ -4738,7 +4701,7 @@
     </row>
     <row r="11" customFormat="false" ht="37.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="21" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="6" t="s">
@@ -4809,94 +4772,94 @@
       <c r="A12" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="E12" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="F12" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="G12" s="33" t="n">
-        <v>3</v>
-      </c>
-      <c r="H12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="I12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="J12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="K12" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="L12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="M12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="N12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="O12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="P12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="R12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="S12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="T12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="U12" s="34" t="n">
-        <v>3</v>
-      </c>
-      <c r="V12" s="35" t="n">
-        <v>3</v>
-      </c>
-      <c r="W12" s="36" t="n">
+      <c r="D12" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="E12" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="F12" s="29" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="T12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="32" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="32" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="20"/>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="C13" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="F13" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="39" t="n">
+      <c r="D13" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="34" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="35" t="n">
         <v>1</v>
       </c>
       <c r="I13" s="25" t="n">
@@ -4905,67 +4868,67 @@
       <c r="J13" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="K13" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="M13" s="39" t="n">
+      <c r="K13" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="M13" s="35" t="n">
         <v>1</v>
       </c>
       <c r="N13" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="O13" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="P13" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="R13" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="S13" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="T13" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="U13" s="39" t="n">
-        <v>1</v>
-      </c>
-      <c r="V13" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="W13" s="40" t="n">
+      <c r="O13" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="P13" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="R13" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="S13" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="T13" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="U13" s="35" t="n">
+        <v>1</v>
+      </c>
+      <c r="V13" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="W13" s="24" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="33.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="20"/>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="E14" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="F14" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="G14" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" s="39" t="n">
+      <c r="D14" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F14" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G14" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="35" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="25" t="n">
@@ -4974,40 +4937,40 @@
       <c r="J14" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="K14" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="L14" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="M14" s="39" t="n">
+      <c r="K14" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="L14" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="M14" s="35" t="n">
         <v>2</v>
       </c>
       <c r="N14" s="25" t="n">
         <v>2</v>
       </c>
-      <c r="O14" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="P14" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="R14" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="S14" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="T14" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="U14" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="V14" s="29" t="n">
+      <c r="O14" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="P14" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="R14" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="S14" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="T14" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="U14" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="V14" s="27" t="n">
         <v>2</v>
       </c>
       <c r="W14" s="22" t="n">
@@ -5015,98 +4978,98 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="36.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="36" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="0" t="n">
         <f aca="false">SUM(D3:D14)</f>
         <v>27</v>
       </c>
-      <c r="E15" s="42" t="n">
+      <c r="E15" s="37" t="n">
         <f aca="false">D15-($D$15/19)</f>
         <v>25.5789473684211</v>
       </c>
-      <c r="F15" s="42" t="n">
+      <c r="F15" s="37" t="n">
         <f aca="false">E15-($D$15/19)</f>
         <v>24.1578947368421</v>
       </c>
-      <c r="G15" s="42" t="n">
+      <c r="G15" s="37" t="n">
         <f aca="false">F15-($D$15/19)</f>
         <v>22.7368421052632</v>
       </c>
-      <c r="H15" s="42" t="n">
+      <c r="H15" s="37" t="n">
         <f aca="false">G15-($D$15/19)</f>
         <v>21.3157894736842</v>
       </c>
-      <c r="I15" s="42" t="n">
+      <c r="I15" s="37" t="n">
         <f aca="false">H15-($D$15/19)</f>
         <v>19.8947368421053</v>
       </c>
-      <c r="J15" s="42" t="n">
+      <c r="J15" s="37" t="n">
         <f aca="false">I15-($D$15/19)</f>
         <v>18.4736842105263</v>
       </c>
-      <c r="K15" s="42" t="n">
+      <c r="K15" s="37" t="n">
         <f aca="false">J15-($D$15/19)</f>
         <v>17.0526315789474</v>
       </c>
-      <c r="L15" s="42" t="n">
+      <c r="L15" s="37" t="n">
         <f aca="false">K15-($D$15/19)</f>
         <v>15.6315789473684</v>
       </c>
-      <c r="M15" s="42" t="n">
+      <c r="M15" s="37" t="n">
         <f aca="false">L15-($D$15/19)</f>
         <v>14.2105263157895</v>
       </c>
-      <c r="N15" s="42" t="n">
+      <c r="N15" s="37" t="n">
         <f aca="false">M15-($D$15/19)</f>
         <v>12.7894736842105</v>
       </c>
-      <c r="O15" s="42" t="n">
+      <c r="O15" s="37" t="n">
         <f aca="false">N15-($D$15/19)</f>
         <v>11.3684210526316</v>
       </c>
-      <c r="P15" s="42" t="n">
+      <c r="P15" s="37" t="n">
         <f aca="false">O15-($D$15/19)</f>
         <v>9.94736842105263</v>
       </c>
-      <c r="Q15" s="42" t="n">
+      <c r="Q15" s="37" t="n">
         <f aca="false">P15-($D$15/19)</f>
         <v>8.52631578947368</v>
       </c>
-      <c r="R15" s="42" t="n">
+      <c r="R15" s="37" t="n">
         <f aca="false">Q15-($D$15/19)</f>
         <v>7.10526315789473</v>
       </c>
-      <c r="S15" s="42" t="n">
+      <c r="S15" s="37" t="n">
         <f aca="false">R15-($D$15/19)</f>
         <v>5.68421052631578</v>
       </c>
-      <c r="T15" s="42" t="n">
+      <c r="T15" s="37" t="n">
         <f aca="false">S15-($D$15/19)</f>
         <v>4.26315789473684</v>
       </c>
-      <c r="U15" s="42" t="n">
+      <c r="U15" s="37" t="n">
         <f aca="false">T15-($D$15/19)</f>
         <v>2.84210526315789</v>
       </c>
-      <c r="V15" s="42" t="n">
+      <c r="V15" s="37" t="n">
         <f aca="false">U15-($D$15/19)</f>
         <v>1.42105263157894</v>
       </c>
-      <c r="W15" s="42" t="n">
+      <c r="W15" s="37" t="n">
         <f aca="false">V15-($D$15/19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="34.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="41"/>
-      <c r="C16" s="41"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
       <c r="D16" s="0" t="n">
         <f aca="false">SUM(D3:D14)</f>
         <v>27</v>
@@ -5121,67 +5084,67 @@
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">SUM(G3:G14)</f>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">SUM(H3:H14)</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I16" s="0" t="n">
         <f aca="false">SUM(I3:I14)</f>
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J16" s="0" t="n">
         <f aca="false">SUM(J3:J14)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K16" s="0" t="n">
         <f aca="false">SUM(K3:K14)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="L16" s="0" t="n">
         <f aca="false">SUM(L3:L14)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="M16" s="0" t="n">
         <f aca="false">SUM(M3:M14)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="N16" s="0" t="n">
         <f aca="false">SUM(N3:N14)</f>
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="O16" s="0" t="n">
         <f aca="false">SUM(O3:O14)</f>
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P16" s="0" t="n">
         <f aca="false">SUM(P3:P14)</f>
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="Q16" s="0" t="n">
         <f aca="false">SUM(Q3:Q14)</f>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="R16" s="0" t="n">
         <f aca="false">SUM(R3:R14)</f>
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="S16" s="0" t="n">
         <f aca="false">SUM(S3:S14)</f>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="T16" s="0" t="n">
         <f aca="false">SUM(T3:T14)</f>
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="U16" s="0" t="n">
         <f aca="false">SUM(U3:U14)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="V16" s="0" t="n">
         <f aca="false">SUM(V3:V14)</f>
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="W16" s="0" t="n">
         <f aca="false">SUM(W3:W14)</f>
@@ -5213,16 +5176,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AR15"/>
+  <dimension ref="A1:AR14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W8" activeCellId="0" sqref="O8:W8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.165991902834"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4372469635628"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.1943319838057"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="9.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.2105263157895"/>
     <col collapsed="false" hidden="false" max="13" min="6" style="0" width="9.1417004048583"/>
@@ -5314,263 +5277,352 @@
       <c r="A2" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="21" t="s">
         <v>60</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="H2" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="K2" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="L2" s="29" t="n">
-        <v>2</v>
-      </c>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
-      <c r="P2" s="29"/>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="22"/>
-    </row>
-    <row r="3" customFormat="false" ht="33.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>3</v>
+      </c>
+      <c r="H2" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="J2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="K2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="L2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="N2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="O2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="P2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="R2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="S2" s="27" t="n">
+        <v>3</v>
+      </c>
+      <c r="T2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="U2" s="27" t="n">
+        <v>2</v>
+      </c>
+      <c r="V2" s="27" t="n">
+        <v>1</v>
+      </c>
+      <c r="W2" s="22" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="20"/>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="F3" s="23" t="n">
-        <v>3</v>
-      </c>
-      <c r="G3" s="6" t="n">
-        <v>3</v>
-      </c>
-      <c r="H3" s="0" t="n">
-        <v>3</v>
+      <c r="D3" s="34" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="34" t="n">
+        <v>4</v>
+      </c>
+      <c r="F3" s="34" t="n">
+        <v>4</v>
+      </c>
+      <c r="G3" s="34" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" s="25" t="n">
+        <v>4</v>
       </c>
       <c r="I3" s="25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J3" s="25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K3" s="25" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L3" s="25" t="n">
-        <v>3</v>
-      </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-    </row>
-    <row r="4" customFormat="false" ht="34.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="M3" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="N3" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="O3" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="P3" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="25" t="n">
+        <v>5</v>
+      </c>
+      <c r="R3" s="25" t="n">
+        <v>5</v>
+      </c>
+      <c r="S3" s="25" t="n">
+        <v>5</v>
+      </c>
+      <c r="T3" s="25" t="n">
+        <v>3</v>
+      </c>
+      <c r="U3" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="W3" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="25.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="20"/>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="E4" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="F4" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="G4" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="H4" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="L4" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="24"/>
-    </row>
-    <row r="5" customFormat="false" ht="25.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C4" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W4" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="21"/>
+    </row>
+    <row r="5" customFormat="false" ht="33.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="20"/>
       <c r="B5" s="21" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="F5" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="H5" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="J5" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="L5" s="23" t="n">
+        <v>2</v>
+      </c>
+      <c r="M5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W5" s="21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="25.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="20"/>
+      <c r="B6" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="W5" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="21"/>
-    </row>
-    <row r="6" customFormat="false" ht="33.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="20"/>
-      <c r="B6" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>23</v>
-      </c>
       <c r="D6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="E6" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="K6" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="L6" s="23" t="n">
-        <v>2</v>
-      </c>
-      <c r="M6" s="21"/>
-      <c r="N6" s="21"/>
-      <c r="O6" s="21"/>
-      <c r="P6" s="21"/>
-      <c r="Q6" s="21"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="21"/>
-      <c r="T6" s="21"/>
-      <c r="U6" s="21"/>
-      <c r="V6" s="21"/>
-      <c r="W6" s="21"/>
-    </row>
-    <row r="7" customFormat="false" ht="25.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="M6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="N6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="P6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="U6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="21"/>
+    </row>
+    <row r="7" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="20"/>
       <c r="B7" s="21" t="s">
         <v>65</v>
@@ -5579,639 +5631,635 @@
         <v>25</v>
       </c>
       <c r="D7" s="6" t="n">
-        <v>2</v>
-      </c>
-      <c r="E7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="T7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="V7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="21"/>
-    </row>
-    <row r="8" customFormat="false" ht="26.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="20"/>
-      <c r="B8" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V7" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="24" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="29" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="M8" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="N8" s="30" t="n">
+        <v>2</v>
+      </c>
+      <c r="O8" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="P8" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="R8" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="S8" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="T8" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="U8" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="V8" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="W8" s="31" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="20"/>
+      <c r="B9" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="25" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="S8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="T8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="U8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V8" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="W8" s="24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="E9" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="F9" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="33" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" s="34" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" s="34" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" s="34" t="n">
-        <v>2</v>
-      </c>
-      <c r="K9" s="35" t="n">
-        <v>2</v>
-      </c>
-      <c r="L9" s="34" t="n">
-        <v>2</v>
-      </c>
-      <c r="M9" s="34"/>
-      <c r="N9" s="34"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="34"/>
-      <c r="Q9" s="34"/>
-      <c r="R9" s="34"/>
-      <c r="S9" s="34"/>
-      <c r="T9" s="34"/>
-      <c r="U9" s="34"/>
-      <c r="V9" s="35"/>
-      <c r="W9" s="36"/>
+      <c r="D9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H9" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="K9" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="L9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W9" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="34"/>
+      <c r="Z9" s="34"/>
+      <c r="AA9" s="34"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="35"/>
+      <c r="AD9" s="35"/>
+      <c r="AE9" s="35"/>
+      <c r="AF9" s="25"/>
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="35"/>
+      <c r="AI9" s="35"/>
+      <c r="AJ9" s="35"/>
+      <c r="AK9" s="35"/>
+      <c r="AL9" s="35"/>
+      <c r="AM9" s="35"/>
+      <c r="AN9" s="35"/>
+      <c r="AO9" s="35"/>
+      <c r="AP9" s="35"/>
+      <c r="AQ9" s="25"/>
+      <c r="AR9" s="24"/>
     </row>
     <row r="10" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="20"/>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="E10" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="F10" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="G10" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="I10" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="L10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="S10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="T10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="U10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="W10" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="X10" s="38"/>
-      <c r="Y10" s="38"/>
-      <c r="Z10" s="38"/>
-      <c r="AA10" s="38"/>
-      <c r="AB10" s="38"/>
-      <c r="AC10" s="39"/>
-      <c r="AD10" s="39"/>
-      <c r="AE10" s="39"/>
-      <c r="AF10" s="28"/>
-      <c r="AG10" s="39"/>
-      <c r="AH10" s="39"/>
-      <c r="AI10" s="39"/>
-      <c r="AJ10" s="39"/>
-      <c r="AK10" s="39"/>
-      <c r="AL10" s="39"/>
-      <c r="AM10" s="39"/>
-      <c r="AN10" s="39"/>
-      <c r="AO10" s="39"/>
-      <c r="AP10" s="39"/>
-      <c r="AQ10" s="28"/>
-      <c r="AR10" s="40"/>
+      <c r="C10" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="L10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="M10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="N10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="O10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="P10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="R10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="S10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="T10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="U10" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="V10" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="W10" s="25" t="n">
+        <v>1</v>
+      </c>
+      <c r="X10" s="34"/>
+      <c r="Y10" s="34"/>
+      <c r="Z10" s="34"/>
+      <c r="AA10" s="34"/>
+      <c r="AB10" s="34"/>
+      <c r="AC10" s="35"/>
+      <c r="AD10" s="35"/>
+      <c r="AE10" s="35"/>
+      <c r="AF10" s="25"/>
+      <c r="AG10" s="35"/>
+      <c r="AH10" s="35"/>
+      <c r="AI10" s="35"/>
+      <c r="AJ10" s="35"/>
+      <c r="AK10" s="35"/>
+      <c r="AL10" s="35"/>
+      <c r="AM10" s="35"/>
+      <c r="AN10" s="35"/>
+      <c r="AO10" s="35"/>
+      <c r="AP10" s="35"/>
+      <c r="AQ10" s="25"/>
+      <c r="AR10" s="24"/>
     </row>
     <row r="11" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="20"/>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="F11" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="G11" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="I11" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="K11" s="28" t="n">
-        <v>2</v>
-      </c>
-      <c r="L11" s="25" t="n">
-        <v>2</v>
-      </c>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
-      <c r="O11" s="24"/>
-      <c r="P11" s="24"/>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="24"/>
-      <c r="S11" s="24"/>
-      <c r="T11" s="24"/>
-      <c r="U11" s="24"/>
-      <c r="V11" s="24"/>
-      <c r="W11" s="24"/>
-      <c r="X11" s="38"/>
-      <c r="Y11" s="38"/>
-      <c r="Z11" s="38"/>
-      <c r="AA11" s="38"/>
-      <c r="AB11" s="38"/>
-      <c r="AC11" s="39"/>
-      <c r="AD11" s="39"/>
-      <c r="AE11" s="39"/>
-      <c r="AF11" s="28"/>
-      <c r="AG11" s="39"/>
-      <c r="AH11" s="39"/>
-      <c r="AI11" s="39"/>
-      <c r="AJ11" s="39"/>
-      <c r="AK11" s="39"/>
-      <c r="AL11" s="39"/>
-      <c r="AM11" s="39"/>
-      <c r="AN11" s="39"/>
-      <c r="AO11" s="39"/>
-      <c r="AP11" s="39"/>
-      <c r="AQ11" s="28"/>
-      <c r="AR11" s="40"/>
+      <c r="C11" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="F11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="G11" s="34" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="K11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="T11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="U11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="V11" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="W11" s="24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="20"/>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="C12" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="E12" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="F12" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="G12" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="H12" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="I12" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="J12" s="39" t="n">
-        <v>2</v>
-      </c>
-      <c r="K12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="P12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="R12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="S12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="T12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="U12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="V12" s="24" t="n">
-        <v>0</v>
-      </c>
-      <c r="W12" s="24" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="20"/>
-      <c r="B13" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="46" t="s">
+      <c r="C12" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="46" t="n">
-        <v>2</v>
-      </c>
-      <c r="E13" s="46" t="n">
-        <v>2</v>
-      </c>
-      <c r="F13" s="46" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="46" t="n">
-        <v>2</v>
-      </c>
-      <c r="H13" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="I13" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="J13" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="K13" s="48" t="n">
-        <v>2</v>
-      </c>
-      <c r="L13" s="47" t="n">
-        <v>2</v>
-      </c>
-      <c r="M13" s="47"/>
-      <c r="N13" s="47"/>
-      <c r="O13" s="47"/>
-      <c r="P13" s="47"/>
-      <c r="Q13" s="47"/>
-      <c r="R13" s="47"/>
-      <c r="S13" s="47"/>
-      <c r="T13" s="47"/>
-      <c r="U13" s="47"/>
-      <c r="V13" s="48"/>
-      <c r="W13" s="49"/>
+      <c r="D12" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="F12" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="G12" s="41" t="n">
+        <v>2</v>
+      </c>
+      <c r="H12" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="J12" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="K12" s="43" t="n">
+        <v>2</v>
+      </c>
+      <c r="L12" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="M12" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="N12" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="O12" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="P12" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="42" t="n">
+        <v>2</v>
+      </c>
+      <c r="R12" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="S12" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="T12" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="U12" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="V12" s="44" t="n">
+        <v>0</v>
+      </c>
+      <c r="W12" s="44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="0" t="n">
+        <f aca="false">SUM(D2:D12)</f>
+        <v>24</v>
+      </c>
+      <c r="E13" s="37" t="n">
+        <f aca="false">D13-($D$13/19)</f>
+        <v>22.7368421052632</v>
+      </c>
+      <c r="F13" s="37" t="n">
+        <f aca="false">E13-($D$13/19)</f>
+        <v>21.4736842105263</v>
+      </c>
+      <c r="G13" s="37" t="n">
+        <f aca="false">F13-($D$13/19)</f>
+        <v>20.2105263157895</v>
+      </c>
+      <c r="H13" s="37" t="n">
+        <f aca="false">G13-($D$13/19)</f>
+        <v>18.9473684210526</v>
+      </c>
+      <c r="I13" s="37" t="n">
+        <f aca="false">H13-($D$13/19)</f>
+        <v>17.6842105263158</v>
+      </c>
+      <c r="J13" s="37" t="n">
+        <f aca="false">I13-($D$13/19)</f>
+        <v>16.4210526315789</v>
+      </c>
+      <c r="K13" s="37" t="n">
+        <f aca="false">J13-($D$13/19)</f>
+        <v>15.1578947368421</v>
+      </c>
+      <c r="L13" s="37" t="n">
+        <f aca="false">K13-($D$13/19)</f>
+        <v>13.8947368421053</v>
+      </c>
+      <c r="M13" s="37" t="n">
+        <f aca="false">L13-($D$13/19)</f>
+        <v>12.6315789473684</v>
+      </c>
+      <c r="N13" s="37" t="n">
+        <f aca="false">M13-($D$13/19)</f>
+        <v>11.3684210526316</v>
+      </c>
+      <c r="O13" s="37" t="n">
+        <f aca="false">N13-($D$13/19)</f>
+        <v>10.1052631578947</v>
+      </c>
+      <c r="P13" s="37" t="n">
+        <f aca="false">O13-($D$13/19)</f>
+        <v>8.84210526315789</v>
+      </c>
+      <c r="Q13" s="37" t="n">
+        <f aca="false">P13-($D$13/19)</f>
+        <v>7.57894736842105</v>
+      </c>
+      <c r="R13" s="37" t="n">
+        <f aca="false">Q13-($D$13/19)</f>
+        <v>6.31578947368421</v>
+      </c>
+      <c r="S13" s="37" t="n">
+        <f aca="false">R13-($D$13/19)</f>
+        <v>5.05263157894736</v>
+      </c>
+      <c r="T13" s="37" t="n">
+        <f aca="false">S13-($D$13/19)</f>
+        <v>3.78947368421052</v>
+      </c>
+      <c r="U13" s="37" t="n">
+        <f aca="false">T13-($D$13/19)</f>
+        <v>2.52631578947368</v>
+      </c>
+      <c r="V13" s="37" t="n">
+        <f aca="false">U13-($D$13/19)</f>
+        <v>1.26315789473684</v>
+      </c>
+      <c r="W13" s="37" t="n">
+        <f aca="false">V13-($D$13/19)</f>
+        <v>-5.32907051820075E-015</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
+      <c r="A14" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
       <c r="D14" s="0" t="n">
-        <f aca="false">SUM(D2:D13)</f>
+        <f aca="false">SUM(D2:D12)</f>
         <v>24</v>
       </c>
-      <c r="E14" s="42" t="n">
-        <f aca="false">D14-($D$14/19)</f>
-        <v>22.7368421052632</v>
-      </c>
-      <c r="F14" s="42" t="n">
-        <f aca="false">E14-($D$14/19)</f>
-        <v>21.4736842105263</v>
-      </c>
-      <c r="G14" s="42" t="n">
-        <f aca="false">F14-($D$14/19)</f>
-        <v>20.2105263157895</v>
-      </c>
-      <c r="H14" s="42" t="n">
-        <f aca="false">G14-($D$14/19)</f>
-        <v>18.9473684210526</v>
-      </c>
-      <c r="I14" s="42" t="n">
-        <f aca="false">H14-($D$14/19)</f>
-        <v>17.6842105263158</v>
-      </c>
-      <c r="J14" s="42" t="n">
-        <f aca="false">I14-($D$14/19)</f>
-        <v>16.4210526315789</v>
-      </c>
-      <c r="K14" s="42" t="n">
-        <f aca="false">J14-($D$14/19)</f>
-        <v>15.1578947368421</v>
-      </c>
-      <c r="L14" s="42" t="n">
-        <f aca="false">K14-($D$14/19)</f>
-        <v>13.8947368421053</v>
-      </c>
-      <c r="M14" s="42" t="n">
-        <f aca="false">L14-($D$14/19)</f>
-        <v>12.6315789473684</v>
-      </c>
-      <c r="N14" s="42" t="n">
-        <f aca="false">M14-($D$14/19)</f>
-        <v>11.3684210526316</v>
-      </c>
-      <c r="O14" s="42" t="n">
-        <f aca="false">N14-($D$14/19)</f>
-        <v>10.1052631578947</v>
-      </c>
-      <c r="P14" s="42" t="n">
-        <f aca="false">O14-($D$14/19)</f>
-        <v>8.84210526315789</v>
-      </c>
-      <c r="Q14" s="42" t="n">
-        <f aca="false">P14-($D$14/19)</f>
-        <v>7.57894736842105</v>
-      </c>
-      <c r="R14" s="42" t="n">
-        <f aca="false">Q14-($D$14/19)</f>
-        <v>6.31578947368421</v>
-      </c>
-      <c r="S14" s="42" t="n">
-        <f aca="false">R14-($D$14/19)</f>
-        <v>5.05263157894736</v>
-      </c>
-      <c r="T14" s="42" t="n">
-        <f aca="false">S14-($D$14/19)</f>
-        <v>3.78947368421052</v>
-      </c>
-      <c r="U14" s="42" t="n">
-        <f aca="false">T14-($D$14/19)</f>
-        <v>2.52631578947368</v>
-      </c>
-      <c r="V14" s="42" t="n">
-        <f aca="false">U14-($D$14/19)</f>
-        <v>1.26315789473684</v>
-      </c>
-      <c r="W14" s="42" t="n">
-        <f aca="false">V14-($D$14/19)</f>
-        <v>-5.32907051820075E-015</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="41" t="s">
-        <v>45</v>
-      </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="0" t="n">
-        <f aca="false">SUM(D2:D13)</f>
-        <v>24</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <f aca="false">SUM(E2:E13)</f>
+      <c r="E14" s="0" t="n">
+        <f aca="false">SUM(E2:E12)</f>
         <v>20</v>
       </c>
-      <c r="F15" s="0" t="n">
-        <f aca="false">SUM(F2:F13)</f>
+      <c r="F14" s="0" t="n">
+        <f aca="false">SUM(F2:F12)</f>
         <v>20</v>
       </c>
-      <c r="G15" s="0" t="n">
-        <f aca="false">SUM(G2:G13)</f>
+      <c r="G14" s="0" t="n">
+        <f aca="false">SUM(G2:G12)</f>
         <v>20</v>
       </c>
-      <c r="H15" s="0" t="n">
-        <f aca="false">SUM(H2:H13)</f>
+      <c r="H14" s="0" t="n">
+        <f aca="false">SUM(H2:H12)</f>
         <v>20</v>
       </c>
-      <c r="I15" s="0" t="n">
-        <f aca="false">SUM(I2:I13)</f>
+      <c r="I14" s="0" t="n">
+        <f aca="false">SUM(I2:I12)</f>
         <v>20</v>
       </c>
-      <c r="J15" s="0" t="n">
-        <f aca="false">SUM(J2:J13)</f>
-        <v>19</v>
-      </c>
-      <c r="K15" s="0" t="n">
-        <f aca="false">SUM(K2:K13)</f>
-        <v>17</v>
-      </c>
-      <c r="L15" s="0" t="n">
-        <f aca="false">SUM(L2:L13)</f>
-        <v>15</v>
-      </c>
-      <c r="M15" s="0" t="n">
-        <f aca="false">SUM(M2:M13)</f>
-        <v>0</v>
-      </c>
-      <c r="N15" s="0" t="n">
-        <f aca="false">SUM(N2:N13)</f>
-        <v>0</v>
-      </c>
-      <c r="O15" s="0" t="n">
-        <f aca="false">SUM(O2:O13)</f>
-        <v>0</v>
-      </c>
-      <c r="P15" s="0" t="n">
-        <f aca="false">SUM(P2:P13)</f>
-        <v>0</v>
-      </c>
-      <c r="Q15" s="0" t="n">
-        <f aca="false">SUM(Q2:Q13)</f>
-        <v>0</v>
-      </c>
-      <c r="R15" s="0" t="n">
-        <f aca="false">SUM(R2:R13)</f>
-        <v>0</v>
-      </c>
-      <c r="S15" s="0" t="n">
-        <f aca="false">SUM(S2:S13)</f>
-        <v>0</v>
-      </c>
-      <c r="T15" s="0" t="n">
-        <f aca="false">SUM(T2:T13)</f>
-        <v>0</v>
-      </c>
-      <c r="U15" s="0" t="n">
-        <f aca="false">SUM(U2:U13)</f>
-        <v>0</v>
-      </c>
-      <c r="V15" s="0" t="n">
-        <f aca="false">SUM(V2:V13)</f>
-        <v>0</v>
-      </c>
-      <c r="W15" s="0" t="n">
-        <f aca="false">SUM(W2:W13)</f>
-        <v>0</v>
+      <c r="J14" s="0" t="n">
+        <f aca="false">SUM(J2:J12)</f>
+        <v>18</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <f aca="false">SUM(K2:K12)</f>
+        <v>16</v>
+      </c>
+      <c r="L14" s="0" t="n">
+        <f aca="false">SUM(L2:L12)</f>
+        <v>14</v>
+      </c>
+      <c r="M14" s="0" t="n">
+        <f aca="false">SUM(M2:M12)</f>
+        <v>12</v>
+      </c>
+      <c r="N14" s="0" t="n">
+        <f aca="false">SUM(N2:N12)</f>
+        <v>12</v>
+      </c>
+      <c r="O14" s="0" t="n">
+        <f aca="false">SUM(O2:O12)</f>
+        <v>12</v>
+      </c>
+      <c r="P14" s="0" t="n">
+        <f aca="false">SUM(P2:P12)</f>
+        <v>12</v>
+      </c>
+      <c r="Q14" s="0" t="n">
+        <f aca="false">SUM(Q2:Q12)</f>
+        <v>13</v>
+      </c>
+      <c r="R14" s="0" t="n">
+        <f aca="false">SUM(R2:R12)</f>
+        <v>12</v>
+      </c>
+      <c r="S14" s="0" t="n">
+        <f aca="false">SUM(S2:S12)</f>
+        <v>13</v>
+      </c>
+      <c r="T14" s="0" t="n">
+        <f aca="false">SUM(T2:T12)</f>
+        <v>9</v>
+      </c>
+      <c r="U14" s="0" t="n">
+        <f aca="false">SUM(U2:U12)</f>
+        <v>8</v>
+      </c>
+      <c r="V14" s="0" t="n">
+        <f aca="false">SUM(V2:V12)</f>
+        <v>5</v>
+      </c>
+      <c r="W14" s="0" t="n">
+        <f aca="false">SUM(W2:W12)</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A2:A8"/>
-    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:C13"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>